<commit_message>
added multiple html files option and cleaned up some
</commit_message>
<xml_diff>
--- a/webapp/data.xlsx
+++ b/webapp/data.xlsx
@@ -513,7 +513,7 @@
         <v>0.6862360802795323</v>
       </c>
       <c r="N2" t="n">
-        <v>0.3009889000000001</v>
+        <v>0.5078755999999984</v>
       </c>
       <c r="O2" t="n">
         <v>7.082991651314155</v>
@@ -540,7 +540,7 @@
         <v>59.77815053634509</v>
       </c>
       <c r="X2" t="n">
-        <v>0.2485722000000017</v>
+        <v>0.2486348000000014</v>
       </c>
     </row>
     <row r="3">
@@ -581,7 +581,7 @@
         <v>0.7673652258821591</v>
       </c>
       <c r="N3" t="n">
-        <v>0.3303395999999985</v>
+        <v>0.4992128000000022</v>
       </c>
       <c r="O3" t="n">
         <v>12.49761708641468</v>
@@ -608,7 +608,7 @@
         <v>35.32730948059873</v>
       </c>
       <c r="X3" t="n">
-        <v>0.2334905999999997</v>
+        <v>0.193343899999995</v>
       </c>
     </row>
     <row r="4">
@@ -649,7 +649,7 @@
         <v>0.7502997363077025</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2624519999999997</v>
+        <v>0.2716589000000056</v>
       </c>
     </row>
     <row r="5">
@@ -690,7 +690,7 @@
         <v>0.7371263675609472</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2012536000000011</v>
+        <v>0.2504936999999998</v>
       </c>
     </row>
     <row r="6">
@@ -734,7 +734,7 @@
         <v>14.9363833160678</v>
       </c>
       <c r="X6" t="n">
-        <v>0.3065415999999992</v>
+        <v>0.2878898999999961</v>
       </c>
     </row>
     <row r="7">
@@ -775,7 +775,7 @@
         <v>0.7294000163856171</v>
       </c>
       <c r="N7" t="n">
-        <v>0.3937162999999977</v>
+        <v>0.5449338000000026</v>
       </c>
       <c r="O7" t="n">
         <v>14.10479914623658</v>
@@ -802,7 +802,7 @@
         <v>55.81376649103811</v>
       </c>
       <c r="X7" t="n">
-        <v>0.4729748000000029</v>
+        <v>0.4270886000000047</v>
       </c>
     </row>
     <row r="8">
@@ -846,7 +846,7 @@
         <v>21.30428090617795</v>
       </c>
       <c r="X8" t="n">
-        <v>0.2243105000000014</v>
+        <v>0.2266720000000007</v>
       </c>
     </row>
     <row r="9">
@@ -921,7 +921,7 @@
         <v>0.6518587763807507</v>
       </c>
       <c r="N11" t="n">
-        <v>0.2131321999999969</v>
+        <v>0.2583630999999968</v>
       </c>
       <c r="O11" t="n">
         <v>8.201533682899196</v>
@@ -948,7 +948,7 @@
         <v>39.23836609572476</v>
       </c>
       <c r="X11" t="n">
-        <v>0.2504792000000009</v>
+        <v>0.2176544000000007</v>
       </c>
     </row>
     <row r="12">
@@ -992,7 +992,7 @@
         <v>22.93589661346448</v>
       </c>
       <c r="X12" t="n">
-        <v>0.1740587000000033</v>
+        <v>0.2033862999999982</v>
       </c>
     </row>
     <row r="13">
@@ -1036,7 +1036,7 @@
         <v>28.22636892663138</v>
       </c>
       <c r="X13" t="n">
-        <v>0.1718703000000019</v>
+        <v>0.2045219000000031</v>
       </c>
     </row>
     <row r="14">
@@ -1080,7 +1080,7 @@
         <v>45.51440616972206</v>
       </c>
       <c r="X14" t="n">
-        <v>0.1595259000000055</v>
+        <v>0.1755707000000015</v>
       </c>
     </row>
     <row r="15">
@@ -1121,7 +1121,7 @@
         <v>0.6343865750227973</v>
       </c>
       <c r="N15" t="n">
-        <v>0.2657932999999986</v>
+        <v>0.4033848000000049</v>
       </c>
       <c r="O15" t="n">
         <v>6.582434431888892</v>
@@ -1148,7 +1148,7 @@
         <v>33.0877576669921</v>
       </c>
       <c r="X15" t="n">
-        <v>0.8409826999999979</v>
+        <v>0.8523867999999979</v>
       </c>
     </row>
     <row r="16">
@@ -1189,7 +1189,7 @@
         <v>0.7412171406140956</v>
       </c>
       <c r="N16" t="n">
-        <v>0.1910053000000005</v>
+        <v>0.2324069999999949</v>
       </c>
       <c r="O16" t="n">
         <v>7.655540733280799</v>
@@ -1216,7 +1216,7 @@
         <v>38.69169951505916</v>
       </c>
       <c r="X16" t="n">
-        <v>0.3414410000000032</v>
+        <v>0.3683844999999977</v>
       </c>
     </row>
     <row r="17">
@@ -1257,7 +1257,7 @@
         <v>0.6174100361520386</v>
       </c>
       <c r="N17" t="n">
-        <v>0.1707388000000023</v>
+        <v>0.1905969000000027</v>
       </c>
       <c r="O17" t="n">
         <v>0.9719154228407159</v>
@@ -1278,7 +1278,7 @@
         <v>8.84430671396882</v>
       </c>
       <c r="X17" t="n">
-        <v>1.1150521</v>
+        <v>0.9703568999999987</v>
       </c>
     </row>
     <row r="18">
@@ -1336,7 +1336,7 @@
         <v>0.7218558184006625</v>
       </c>
       <c r="N19" t="n">
-        <v>0.2235069999999979</v>
+        <v>0.2332853999999998</v>
       </c>
       <c r="O19" t="n">
         <v>6.807915252906037</v>
@@ -1363,7 +1363,7 @@
         <v>46.80842965199952</v>
       </c>
       <c r="X19" t="n">
-        <v>0.4137875999999991</v>
+        <v>0.4081564000000029</v>
       </c>
     </row>
     <row r="20">
@@ -1404,7 +1404,7 @@
         <v>0.5445504221440435</v>
       </c>
       <c r="N20" t="n">
-        <v>0.2915412000000046</v>
+        <v>0.3659639999999982</v>
       </c>
       <c r="O20" t="n">
         <v>8.896998358735726</v>
@@ -1431,7 +1431,7 @@
         <v>55.20376541448184</v>
       </c>
       <c r="X20" t="n">
-        <v>0.1834343999999959</v>
+        <v>0.1779270000000039</v>
       </c>
     </row>
     <row r="21">
@@ -1472,7 +1472,7 @@
         <v>0.6954927850998559</v>
       </c>
       <c r="N21" t="n">
-        <v>0.1707103000000032</v>
+        <v>0.2104149999999976</v>
       </c>
       <c r="O21" t="n">
         <v>3.751261323481207</v>
@@ -1499,7 +1499,7 @@
         <v>39.34970828088581</v>
       </c>
       <c r="X21" t="n">
-        <v>0.2925927000000001</v>
+        <v>0.2939124999999976</v>
       </c>
     </row>
     <row r="22">
@@ -1540,7 +1540,7 @@
         <v>0.7145603697052624</v>
       </c>
       <c r="N22" t="n">
-        <v>0.2606058000000004</v>
+        <v>0.3085018000000019</v>
       </c>
       <c r="O22" t="n">
         <v>9.140000458889755</v>
@@ -1567,7 +1567,7 @@
         <v>57.53614698372837</v>
       </c>
       <c r="X22" t="n">
-        <v>0.1565597999999966</v>
+        <v>0.1623935999999944</v>
       </c>
     </row>
     <row r="23">
@@ -1608,7 +1608,7 @@
         <v>0.7885762479942238</v>
       </c>
       <c r="N23" t="n">
-        <v>0.1454617000000056</v>
+        <v>0.1887624000000017</v>
       </c>
       <c r="O23" t="n">
         <v>2.416074115714946</v>
@@ -1635,7 +1635,7 @@
         <v>35.13999931153762</v>
       </c>
       <c r="X23" t="n">
-        <v>0.140543099999995</v>
+        <v>0.1469149999999999</v>
       </c>
     </row>
     <row r="24">
@@ -1676,7 +1676,7 @@
         <v>0.7673795573162669</v>
       </c>
       <c r="N24" t="n">
-        <v>0.2544101999999953</v>
+        <v>0.3398419999999973</v>
       </c>
       <c r="O24" t="n">
         <v>14.07512366789098</v>
@@ -1703,7 +1703,7 @@
         <v>46.39416756456535</v>
       </c>
       <c r="X24" t="n">
-        <v>0.1731758000000028</v>
+        <v>0.1983905999999962</v>
       </c>
     </row>
     <row r="25">
@@ -1744,7 +1744,7 @@
         <v>0.5893135288182765</v>
       </c>
       <c r="N25" t="n">
-        <v>0.1715687999999957</v>
+        <v>0.2194961999999947</v>
       </c>
     </row>
     <row r="26">
@@ -1785,7 +1785,7 @@
         <v>0.6289246745312014</v>
       </c>
       <c r="N26" t="n">
-        <v>0.2220060000000004</v>
+        <v>0.3090657999999991</v>
       </c>
       <c r="O26" t="n">
         <v>11.84910243788312</v>
@@ -1812,7 +1812,7 @@
         <v>50.2525579907014</v>
       </c>
       <c r="X26" t="n">
-        <v>0.2375982999999948</v>
+        <v>0.2517217999999986</v>
       </c>
     </row>
     <row r="27">
@@ -1870,7 +1870,7 @@
         <v>0.5999804683154401</v>
       </c>
       <c r="N28" t="n">
-        <v>0.2550793000000056</v>
+        <v>0.3078181000000058</v>
       </c>
       <c r="O28" t="n">
         <v>2.786952465828485</v>
@@ -1894,7 +1894,7 @@
         <v>56.59696015007074</v>
       </c>
       <c r="X28" t="n">
-        <v>0.2587242999999972</v>
+        <v>0.2405296999999962</v>
       </c>
     </row>
     <row r="29">
@@ -1935,7 +1935,7 @@
         <v>0.71888906807707</v>
       </c>
       <c r="N29" t="n">
-        <v>0.2956058000000041</v>
+        <v>0.3542256000000066</v>
       </c>
       <c r="O29" t="n">
         <v>5.904264218426784</v>
@@ -1962,7 +1962,7 @@
         <v>51.96646310751828</v>
       </c>
       <c r="X29" t="n">
-        <v>0.7739044999999933</v>
+        <v>0.8636651000000057</v>
       </c>
     </row>
     <row r="30">
@@ -2003,7 +2003,7 @@
         <v>0.5786847596367948</v>
       </c>
       <c r="N30" t="n">
-        <v>0.3615658999999951</v>
+        <v>0.2890650000000079</v>
       </c>
       <c r="O30" t="n">
         <v>13.55025677870883</v>
@@ -2030,7 +2030,7 @@
         <v>58.1407327462955</v>
       </c>
       <c r="X30" t="n">
-        <v>0.2909567999999965</v>
+        <v>0.2889883999999938</v>
       </c>
     </row>
     <row r="31">
@@ -2071,7 +2071,7 @@
         <v>0.6800036212002831</v>
       </c>
       <c r="N31" t="n">
-        <v>0.2700864999999979</v>
+        <v>0.3039978000000048</v>
       </c>
       <c r="O31" t="n">
         <v>9.885791273851719</v>
@@ -2098,7 +2098,7 @@
         <v>36.56763280519203</v>
       </c>
       <c r="X31" t="n">
-        <v>0.2274193000000011</v>
+        <v>0.2087596000000076</v>
       </c>
     </row>
     <row r="32">
@@ -2139,7 +2139,7 @@
         <v>0.8022139622054861</v>
       </c>
       <c r="N32" t="n">
-        <v>0.3482640000000004</v>
+        <v>0.423135000000002</v>
       </c>
       <c r="O32" t="n">
         <v>11.50243435678393</v>
@@ -2166,7 +2166,7 @@
         <v>59.48210624045475</v>
       </c>
       <c r="X32" t="n">
-        <v>0.3280930000000026</v>
+        <v>0.2608871999999991</v>
       </c>
     </row>
     <row r="33">
@@ -2227,7 +2227,7 @@
         <v>50.86138544009225</v>
       </c>
       <c r="X34" t="n">
-        <v>0.3951634000000013</v>
+        <v>0.4242200999999994</v>
       </c>
     </row>
     <row r="35">
@@ -2271,7 +2271,7 @@
         <v>23.18246951406661</v>
       </c>
       <c r="X35" t="n">
-        <v>0.1719992000000019</v>
+        <v>0.1588536000000005</v>
       </c>
     </row>
     <row r="36">
@@ -2315,7 +2315,7 @@
         <v>16.43928921731816</v>
       </c>
       <c r="X36" t="n">
-        <v>0.2179836999999978</v>
+        <v>0.2041973999999982</v>
       </c>
     </row>
     <row r="37">
@@ -2356,7 +2356,7 @@
         <v>0.586159877402691</v>
       </c>
       <c r="N37" t="n">
-        <v>0.2769161999999952</v>
+        <v>0.3063585000000018</v>
       </c>
       <c r="O37" t="n">
         <v>6.954434984205963</v>
@@ -2383,7 +2383,7 @@
         <v>49.846764840275</v>
       </c>
       <c r="X37" t="n">
-        <v>0.1406593000000029</v>
+        <v>0.1518092999999965</v>
       </c>
     </row>
     <row r="38">
@@ -2441,7 +2441,7 @@
         <v>55.54071084240474</v>
       </c>
       <c r="X39" t="n">
-        <v>0.5496080000000063</v>
+        <v>0.5833504000000005</v>
       </c>
     </row>
     <row r="40">
@@ -2482,7 +2482,7 @@
         <v>0.5614734246846576</v>
       </c>
       <c r="N40" t="n">
-        <v>0.5075228999999979</v>
+        <v>0.6307156999999961</v>
       </c>
     </row>
     <row r="41">
@@ -2523,7 +2523,7 @@
         <v>0.952559957246823</v>
       </c>
       <c r="N41" t="n">
-        <v>0.347015600000006</v>
+        <v>0.2490895999999907</v>
       </c>
       <c r="O41" t="n">
         <v>5.77109258684423</v>
@@ -2550,7 +2550,7 @@
         <v>55.33722413506393</v>
       </c>
       <c r="X41" t="n">
-        <v>0.1965205999999995</v>
+        <v>0.1361961000000065</v>
       </c>
     </row>
     <row r="42">
@@ -2591,7 +2591,7 @@
         <v>0.7050371273664621</v>
       </c>
       <c r="N42" t="n">
-        <v>0.2846122999999992</v>
+        <v>0.2546674000000024</v>
       </c>
       <c r="O42" t="n">
         <v>1.075604586092394</v>
@@ -2612,7 +2612,7 @@
         <v>19.74265575570439</v>
       </c>
       <c r="X42" t="n">
-        <v>0.593699799999996</v>
+        <v>0.4596289999999925</v>
       </c>
     </row>
     <row r="43">
@@ -2649,28 +2649,28 @@
         <v>1910</v>
       </c>
       <c r="F44" t="n">
-        <v>7.739296442963667</v>
+        <v>6.543252991091501</v>
       </c>
       <c r="G44" t="n">
-        <v>24.05998894185596</v>
+        <v>20.34171914328964</v>
       </c>
       <c r="H44" t="n">
         <v>3</v>
       </c>
       <c r="I44" t="n">
-        <v>158.3091226190668</v>
+        <v>155.1541375285876</v>
       </c>
       <c r="J44" t="n">
-        <v>0.7752867010950539</v>
+        <v>0.8925476632113988</v>
       </c>
       <c r="K44" t="n">
-        <v>0.9487731589514892</v>
+        <v>0.8925476632113987</v>
       </c>
       <c r="L44" t="n">
-        <v>0.7752867010950539</v>
+        <v>0.8800581615536265</v>
       </c>
       <c r="N44" t="n">
-        <v>0.4280708999999945</v>
+        <v>0.2592863000000136</v>
       </c>
       <c r="O44" t="n">
         <v>9.84163207654866</v>
@@ -2697,7 +2697,7 @@
         <v>40.66306484336559</v>
       </c>
       <c r="X44" t="n">
-        <v>0.5811330000000012</v>
+        <v>0.5271022999999957</v>
       </c>
     </row>
     <row r="45">
@@ -2741,7 +2741,7 @@
         <v>56.30770522182081</v>
       </c>
       <c r="X45" t="n">
-        <v>0.1560862000000043</v>
+        <v>0.1700440999999984</v>
       </c>
     </row>
     <row r="46">
@@ -2785,7 +2785,7 @@
         <v>59.04088714732057</v>
       </c>
       <c r="X46" t="n">
-        <v>0.2818128999999985</v>
+        <v>0.2904535999999922</v>
       </c>
     </row>
     <row r="47">
@@ -2843,7 +2843,7 @@
         <v>0.7881604774505526</v>
       </c>
       <c r="N48" t="n">
-        <v>0.2609574999999964</v>
+        <v>0.2820542000000046</v>
       </c>
       <c r="O48" t="n">
         <v>11.62392031857079</v>
@@ -2870,7 +2870,7 @@
         <v>46.45972825576388</v>
       </c>
       <c r="X48" t="n">
-        <v>0.2616286000000017</v>
+        <v>0.2307234000000022</v>
       </c>
     </row>
     <row r="49">
@@ -2914,7 +2914,7 @@
         <v>59.55296311242046</v>
       </c>
       <c r="X49" t="n">
-        <v>0.3876428000000018</v>
+        <v>0.3866277999999994</v>
       </c>
     </row>
     <row r="50">
@@ -2989,7 +2989,7 @@
         <v>0.7134380378238956</v>
       </c>
       <c r="N52" t="n">
-        <v>0.2618065999999999</v>
+        <v>0.3077657000000045</v>
       </c>
       <c r="O52" t="n">
         <v>13.47114947668005</v>
@@ -3016,7 +3016,7 @@
         <v>47.30506405382903</v>
       </c>
       <c r="X52" t="n">
-        <v>0.2928421999999955</v>
+        <v>0.3021984999999887</v>
       </c>
     </row>
     <row r="53">
@@ -3057,7 +3057,7 @@
         <v>0.7574887991113182</v>
       </c>
       <c r="N53" t="n">
-        <v>0.7736055000000022</v>
+        <v>0.8670225999999985</v>
       </c>
       <c r="O53" t="n">
         <v>11.31119466449514</v>
@@ -3084,7 +3084,7 @@
         <v>48.57156942197514</v>
       </c>
       <c r="X53" t="n">
-        <v>0.2767125999999962</v>
+        <v>0.3409987000000001</v>
       </c>
     </row>
     <row r="54">
@@ -3125,7 +3125,7 @@
         <v>0.7454613074654333</v>
       </c>
       <c r="N54" t="n">
-        <v>0.2027009000000035</v>
+        <v>0.2396370000000019</v>
       </c>
       <c r="O54" t="n">
         <v>11.65213715318634</v>
@@ -3152,7 +3152,7 @@
         <v>38.71382560609396</v>
       </c>
       <c r="X54" t="n">
-        <v>0.2510195000000053</v>
+        <v>0.2324710999999979</v>
       </c>
     </row>
     <row r="55">
@@ -3261,7 +3261,7 @@
         <v>0.5572668092236944</v>
       </c>
       <c r="N59" t="n">
-        <v>0.2601422000000042</v>
+        <v>0.3453062999999901</v>
       </c>
       <c r="O59" t="n">
         <v>13.10461298038586</v>
@@ -3288,7 +3288,7 @@
         <v>42.88304695540518</v>
       </c>
       <c r="X59" t="n">
-        <v>0.2466154000000031</v>
+        <v>0.2468679999999921</v>
       </c>
     </row>
     <row r="60">
@@ -3329,7 +3329,7 @@
         <v>0.6309847701756546</v>
       </c>
       <c r="N60" t="n">
-        <v>0.2508493999999999</v>
+        <v>0.2906928999999963</v>
       </c>
     </row>
     <row r="61">
@@ -3370,7 +3370,7 @@
         <v>0.7867007228834226</v>
       </c>
       <c r="N61" t="n">
-        <v>0.3065685999999985</v>
+        <v>0.303648999999993</v>
       </c>
       <c r="O61" t="n">
         <v>9.987862134498778</v>
@@ -3397,7 +3397,7 @@
         <v>53.77820152627504</v>
       </c>
       <c r="X61" t="n">
-        <v>0.3045866999999944</v>
+        <v>0.2308053999999942</v>
       </c>
     </row>
     <row r="62">
@@ -3441,7 +3441,7 @@
         <v>45.23882636811368</v>
       </c>
       <c r="X62" t="n">
-        <v>0.2097020000000001</v>
+        <v>0.1711808000000019</v>
       </c>
     </row>
     <row r="63">
@@ -3502,7 +3502,7 @@
         <v>37.56753887726268</v>
       </c>
       <c r="X64" t="n">
-        <v>0.2688593000000026</v>
+        <v>0.2929305999999912</v>
       </c>
     </row>
     <row r="65">
@@ -3521,30 +3521,6 @@
       <c r="E65" t="n">
         <v>2114</v>
       </c>
-      <c r="F65" t="n">
-        <v>10.50526734053436</v>
-      </c>
-      <c r="G65" t="n">
-        <v>32.65886219855242</v>
-      </c>
-      <c r="H65" t="n">
-        <v>3</v>
-      </c>
-      <c r="I65" t="n">
-        <v>165.2283969657749</v>
-      </c>
-      <c r="J65" t="n">
-        <v>0.6045626252366123</v>
-      </c>
-      <c r="K65" t="n">
-        <v>0.6582476994966975</v>
-      </c>
-      <c r="L65" t="n">
-        <v>0.7664820620288616</v>
-      </c>
-      <c r="N65" t="n">
-        <v>0.5866030999999978</v>
-      </c>
       <c r="O65" t="n">
         <v>3.509165855753642</v>
       </c>
@@ -3564,7 +3540,7 @@
         <v>48.09420178143387</v>
       </c>
       <c r="X65" t="n">
-        <v>0.5843880999999982</v>
+        <v>0.6782733999999948</v>
       </c>
     </row>
     <row r="66">
@@ -3605,7 +3581,7 @@
         <v>0.9568050625003772</v>
       </c>
       <c r="N66" t="n">
-        <v>0.2397773000000001</v>
+        <v>0.7905114999999938</v>
       </c>
       <c r="O66" t="n">
         <v>8.339759165045479</v>
@@ -3632,7 +3608,7 @@
         <v>35.08335700389608</v>
       </c>
       <c r="X66" t="n">
-        <v>0.3157039999999967</v>
+        <v>1.107742799999997</v>
       </c>
     </row>
     <row r="67">
@@ -3676,7 +3652,7 @@
         <v>57.97587948174441</v>
       </c>
       <c r="X67" t="n">
-        <v>0.1792733999999996</v>
+        <v>0.2037416000000007</v>
       </c>
     </row>
     <row r="68">
@@ -3717,7 +3693,7 @@
         <v>0.7520959774273354</v>
       </c>
       <c r="N68" t="n">
-        <v>0.3815927999999928</v>
+        <v>0.4320928000000066</v>
       </c>
       <c r="O68" t="n">
         <v>12.42246620264435</v>
@@ -3744,7 +3720,7 @@
         <v>29.166953977866</v>
       </c>
       <c r="X68" t="n">
-        <v>0.2595902000000052</v>
+        <v>0.2801455999999973</v>
       </c>
     </row>
     <row r="69">
@@ -3785,7 +3761,7 @@
         <v>0.6859577668551914</v>
       </c>
       <c r="N69" t="n">
-        <v>0.2414595999999989</v>
+        <v>0.3248198000000002</v>
       </c>
     </row>
     <row r="70">
@@ -3843,7 +3819,7 @@
         <v>0.7502103559470656</v>
       </c>
       <c r="N71" t="n">
-        <v>0.3505870999999985</v>
+        <v>0.2855457000000001</v>
       </c>
       <c r="O71" t="n">
         <v>7.572412157140905</v>
@@ -3870,7 +3846,7 @@
         <v>29.13443686836865</v>
       </c>
       <c r="X71" t="n">
-        <v>0.1772519999999957</v>
+        <v>0.1836291000000045</v>
       </c>
     </row>
     <row r="72">
@@ -3928,7 +3904,7 @@
         <v>0.7489480931143536</v>
       </c>
       <c r="N73" t="n">
-        <v>0.2446883000000071</v>
+        <v>0.299043999999995</v>
       </c>
       <c r="O73" t="n">
         <v>15.80939597182488</v>
@@ -3955,7 +3931,7 @@
         <v>53.65016599065109</v>
       </c>
       <c r="X73" t="n">
-        <v>0.2727134000000007</v>
+        <v>0.4593311</v>
       </c>
     </row>
     <row r="74">
@@ -3993,7 +3969,7 @@
         <v>28.6141737287187</v>
       </c>
       <c r="X74" t="n">
-        <v>0.6990232999999932</v>
+        <v>1.09838400000001</v>
       </c>
     </row>
     <row r="75">
@@ -4034,7 +4010,7 @@
         <v>47.40962670901428</v>
       </c>
       <c r="X75" t="n">
-        <v>0.3371881999999999</v>
+        <v>0.4944398999999891</v>
       </c>
     </row>
     <row r="76">
@@ -4075,7 +4051,7 @@
         <v>0.6945818775739012</v>
       </c>
       <c r="N76" t="n">
-        <v>0.2375380000000007</v>
+        <v>0.3176570000000112</v>
       </c>
       <c r="O76" t="n">
         <v>12.09781490595968</v>
@@ -4102,7 +4078,7 @@
         <v>56.38251254024499</v>
       </c>
       <c r="X76" t="n">
-        <v>0.139353799999995</v>
+        <v>0.1836643000000038</v>
       </c>
     </row>
     <row r="77">
@@ -4143,7 +4119,7 @@
         <v>0.765234274966803</v>
       </c>
       <c r="N77" t="n">
-        <v>0.2305972999999994</v>
+        <v>0.3123882000000151</v>
       </c>
       <c r="O77" t="n">
         <v>10.57013802622273</v>
@@ -4170,7 +4146,7 @@
         <v>53.89571795561051</v>
       </c>
       <c r="X77" t="n">
-        <v>0.179326599999996</v>
+        <v>0.209526000000011</v>
       </c>
     </row>
     <row r="78">
@@ -4211,7 +4187,7 @@
         <v>0.6847391850735041</v>
       </c>
       <c r="N78" t="n">
-        <v>0.2784386999999953</v>
+        <v>0.4066971999999964</v>
       </c>
       <c r="O78" t="n">
         <v>11.06833403200247</v>
@@ -4238,7 +4214,7 @@
         <v>40.24225044544824</v>
       </c>
       <c r="X78" t="n">
-        <v>0.2836288000000025</v>
+        <v>0.1887605000000008</v>
       </c>
     </row>
     <row r="79">
@@ -4279,7 +4255,7 @@
         <v>0.7301596146116747</v>
       </c>
       <c r="N79" t="n">
-        <v>0.385137499999999</v>
+        <v>0.4491710000000069</v>
       </c>
     </row>
     <row r="80">
@@ -4354,7 +4330,7 @@
         <v>0.7327754278658019</v>
       </c>
       <c r="N82" t="n">
-        <v>0.1935485000000057</v>
+        <v>0.2529896000000065</v>
       </c>
       <c r="O82" t="n">
         <v>10.61089507863382</v>
@@ -4381,7 +4357,7 @@
         <v>57.9426278929609</v>
       </c>
       <c r="X82" t="n">
-        <v>0.3044857000000007</v>
+        <v>0.3204867999999976</v>
       </c>
     </row>
     <row r="83">
@@ -4422,7 +4398,7 @@
         <v>0.7764527465325202</v>
       </c>
       <c r="N83" t="n">
-        <v>0.3823337999999978</v>
+        <v>0.3613784000000066</v>
       </c>
       <c r="O83" t="n">
         <v>13.04264621425495</v>
@@ -4449,7 +4425,7 @@
         <v>54.41365671433891</v>
       </c>
       <c r="X83" t="n">
-        <v>0.2833246000000003</v>
+        <v>0.3112013999999874</v>
       </c>
     </row>
     <row r="84">
@@ -4490,7 +4466,7 @@
         <v>0.7137209245069888</v>
       </c>
       <c r="N84" t="n">
-        <v>0.2390855000000016</v>
+        <v>0.3214187000000095</v>
       </c>
       <c r="O84" t="n">
         <v>14.26093881179648</v>
@@ -4517,7 +4493,7 @@
         <v>53.64682303198879</v>
       </c>
       <c r="X84" t="n">
-        <v>0.2087728999999996</v>
+        <v>0.2208834999999851</v>
       </c>
     </row>
     <row r="85">
@@ -4561,7 +4537,7 @@
         <v>44.07957798744502</v>
       </c>
       <c r="X85" t="n">
-        <v>0.2198905999999994</v>
+        <v>0.2096298999999817</v>
       </c>
     </row>
     <row r="86">
@@ -4619,7 +4595,7 @@
         <v>0.5196037362405583</v>
       </c>
       <c r="N87" t="n">
-        <v>0.2081433999999973</v>
+        <v>0.2612530000000106</v>
       </c>
       <c r="O87" t="n">
         <v>10.39177272279499</v>
@@ -4646,7 +4622,7 @@
         <v>54.746075089854</v>
       </c>
       <c r="X87" t="n">
-        <v>0.6230519000000072</v>
+        <v>0.7432602000000088</v>
       </c>
     </row>
     <row r="88">
@@ -4687,7 +4663,7 @@
         <v>0.6765364810570895</v>
       </c>
       <c r="N88" t="n">
-        <v>0.1867694999999969</v>
+        <v>0.2313745000000154</v>
       </c>
     </row>
     <row r="89">
@@ -4748,7 +4724,7 @@
         <v>24.87998961051136</v>
       </c>
       <c r="X90" t="n">
-        <v>0.1496570999999989</v>
+        <v>0.1650218000000052</v>
       </c>
     </row>
     <row r="91">
@@ -4840,7 +4816,7 @@
         <v>0.7258996951481946</v>
       </c>
       <c r="N94" t="n">
-        <v>0.2141273000000012</v>
+        <v>0.2591302999999812</v>
       </c>
       <c r="O94" t="n">
         <v>14.34155742807301</v>
@@ -4867,7 +4843,7 @@
         <v>51.00140785089667</v>
       </c>
       <c r="X94" t="n">
-        <v>0.230536100000009</v>
+        <v>0.2326786000000141</v>
       </c>
     </row>
     <row r="95">
@@ -4945,7 +4921,7 @@
         <v>48.63095956622971</v>
       </c>
       <c r="X97" t="n">
-        <v>0.2550619999999952</v>
+        <v>0.2743995000000155</v>
       </c>
     </row>
     <row r="98">
@@ -4986,7 +4962,7 @@
         <v>0.6110729467681992</v>
       </c>
       <c r="N98" t="n">
-        <v>0.2693919999999963</v>
+        <v>0.3396310999999912</v>
       </c>
       <c r="O98" t="n">
         <v>9.03843260641283</v>
@@ -5013,7 +4989,7 @@
         <v>55.84863048047959</v>
       </c>
       <c r="X98" t="n">
-        <v>0.5905721999999969</v>
+        <v>0.5978680999999995</v>
       </c>
     </row>
     <row r="99">
@@ -5054,7 +5030,7 @@
         <v>0.6401584182965168</v>
       </c>
       <c r="N99" t="n">
-        <v>0.253643100000005</v>
+        <v>0.2905568000000187</v>
       </c>
       <c r="O99" t="n">
         <v>5.851133559999255</v>
@@ -5081,7 +5057,7 @@
         <v>42.33478532309601</v>
       </c>
       <c r="X99" t="n">
-        <v>0.2403247000000022</v>
+        <v>0.2516655999999955</v>
       </c>
     </row>
     <row r="100">
@@ -5142,7 +5118,7 @@
         <v>52.66508630199286</v>
       </c>
       <c r="X101" t="n">
-        <v>0.2131589000000105</v>
+        <v>0.1693952999999908</v>
       </c>
     </row>
     <row r="102">
@@ -5183,7 +5159,7 @@
         <v>0.5490618954190731</v>
       </c>
       <c r="N102" t="n">
-        <v>0.2689352000000014</v>
+        <v>0.3196444000000156</v>
       </c>
       <c r="O102" t="n">
         <v>10.4053991511358</v>
@@ -5210,7 +5186,7 @@
         <v>44.84836519228753</v>
       </c>
       <c r="X102" t="n">
-        <v>0.7108889000000005</v>
+        <v>0.7030838999999958</v>
       </c>
     </row>
     <row r="103">
@@ -5251,7 +5227,7 @@
         <v>0.7592616329955325</v>
       </c>
       <c r="N103" t="n">
-        <v>0.1744484999999969</v>
+        <v>0.2144890000000146</v>
       </c>
       <c r="O103" t="n">
         <v>4.792432876864117</v>
@@ -5278,7 +5254,7 @@
         <v>39.9419958169031</v>
       </c>
       <c r="X103" t="n">
-        <v>0.1649859000000049</v>
+        <v>0.1610058999999922</v>
       </c>
     </row>
     <row r="104">
@@ -5322,7 +5298,7 @@
         <v>23.11590132617221</v>
       </c>
       <c r="X104" t="n">
-        <v>0.1900688000000059</v>
+        <v>0.2203796000000011</v>
       </c>
     </row>
     <row r="105">
@@ -5380,7 +5356,7 @@
         <v>0.5630212263897855</v>
       </c>
       <c r="N106" t="n">
-        <v>0.2465897000000012</v>
+        <v>0.2832903999999985</v>
       </c>
       <c r="O106" t="n">
         <v>9.093567248490176</v>
@@ -5407,7 +5383,7 @@
         <v>52.2049780764026</v>
       </c>
       <c r="X106" t="n">
-        <v>0.2328720000000004</v>
+        <v>0.2371751000000017</v>
       </c>
     </row>
     <row r="107">
@@ -5451,7 +5427,7 @@
         <v>58.87600731870526</v>
       </c>
       <c r="X107" t="n">
-        <v>0.3658186999999913</v>
+        <v>0.3948299999999847</v>
       </c>
     </row>
     <row r="108">
@@ -5492,7 +5468,7 @@
         <v>58.65767156528716</v>
       </c>
       <c r="X108" t="n">
-        <v>0.4668367999999958</v>
+        <v>0.5570453999999927</v>
       </c>
     </row>
     <row r="109">
@@ -5530,7 +5506,7 @@
         <v>11.82465668211256</v>
       </c>
       <c r="X109" t="n">
-        <v>0.2786169000000029</v>
+        <v>0.2919445999999937</v>
       </c>
     </row>
     <row r="110">
@@ -5588,7 +5564,7 @@
         <v>0.7693640756993421</v>
       </c>
       <c r="N111" t="n">
-        <v>0.2184117999999984</v>
+        <v>0.2696454000000017</v>
       </c>
       <c r="O111" t="n">
         <v>6.18550542330814</v>
@@ -5612,7 +5588,7 @@
         <v>17.82265020858767</v>
       </c>
       <c r="X111" t="n">
-        <v>0.1953206999999964</v>
+        <v>0.2004991999999959</v>
       </c>
     </row>
     <row r="112">
@@ -5653,7 +5629,7 @@
         <v>0.7072238685633592</v>
       </c>
       <c r="N112" t="n">
-        <v>0.2997230000000002</v>
+        <v>0.353026199999988</v>
       </c>
     </row>
     <row r="113">
@@ -5694,7 +5670,7 @@
         <v>0.563446518934809</v>
       </c>
       <c r="N113" t="n">
-        <v>0.2799545999999964</v>
+        <v>0.2834584999999947</v>
       </c>
     </row>
     <row r="114">
@@ -5735,7 +5711,7 @@
         <v>0.7176673529978116</v>
       </c>
       <c r="N114" t="n">
-        <v>0.256458600000002</v>
+        <v>0.2583320000000242</v>
       </c>
       <c r="O114" t="n">
         <v>13.10792546632432</v>
@@ -5762,7 +5738,7 @@
         <v>54.58696210380293</v>
       </c>
       <c r="X114" t="n">
-        <v>0.2240250000000117</v>
+        <v>0.2251486000000114</v>
       </c>
     </row>
     <row r="115">
@@ -5803,7 +5779,7 @@
         <v>0.6293457841602239</v>
       </c>
       <c r="N115" t="n">
-        <v>0.2916201000000029</v>
+        <v>0.2985704000000169</v>
       </c>
       <c r="O115" t="n">
         <v>9.362845680181721</v>
@@ -5830,7 +5806,7 @@
         <v>53.19096702890215</v>
       </c>
       <c r="X115" t="n">
-        <v>0.3201890999999932</v>
+        <v>0.3020305000000008</v>
       </c>
     </row>
     <row r="116">
@@ -5871,7 +5847,7 @@
         <v>0.6512815729622599</v>
       </c>
       <c r="N116" t="n">
-        <v>0.5558718999999996</v>
+        <v>0.6290228999999954</v>
       </c>
       <c r="O116" t="n">
         <v>12.17253832135357</v>
@@ -5898,7 +5874,7 @@
         <v>41.10830087359403</v>
       </c>
       <c r="X116" t="n">
-        <v>1.173067900000007</v>
+        <v>1.150789299999985</v>
       </c>
     </row>
     <row r="117">
@@ -5959,7 +5935,7 @@
         <v>15.29120368022069</v>
       </c>
       <c r="X118" t="n">
-        <v>0.2475998000000033</v>
+        <v>0.2738549000000035</v>
       </c>
     </row>
     <row r="119">
@@ -6051,7 +6027,7 @@
         <v>0.7853935829475021</v>
       </c>
       <c r="N122" t="n">
-        <v>0.2805833000000035</v>
+        <v>0.3353623000000141</v>
       </c>
       <c r="O122" t="n">
         <v>16.54905738559482</v>
@@ -6078,7 +6054,7 @@
         <v>45.55108687726033</v>
       </c>
       <c r="X122" t="n">
-        <v>0.3663205999999946</v>
+        <v>0.4158081999999865</v>
       </c>
     </row>
     <row r="123">
@@ -6119,7 +6095,7 @@
         <v>0.5550880981211724</v>
       </c>
       <c r="N123" t="n">
-        <v>0.3656681000000077</v>
+        <v>0.4364977999999837</v>
       </c>
       <c r="O123" t="n">
         <v>11.10295649589333</v>
@@ -6146,7 +6122,7 @@
         <v>59.55105576581059</v>
       </c>
       <c r="X123" t="n">
-        <v>0.3133011999999979</v>
+        <v>0.319972899999982</v>
       </c>
     </row>
     <row r="124">
@@ -6207,7 +6183,7 @@
         <v>45.09149429746742</v>
       </c>
       <c r="X125" t="n">
-        <v>0.1365035000000034</v>
+        <v>0.1472372000000064</v>
       </c>
     </row>
     <row r="126">
@@ -6251,7 +6227,7 @@
         <v>53.87732308547976</v>
       </c>
       <c r="X126" t="n">
-        <v>0.3099493999999936</v>
+        <v>0.3331639000000166</v>
       </c>
     </row>
     <row r="127">
@@ -6309,7 +6285,7 @@
         <v>0.7659442343454008</v>
       </c>
       <c r="N128" t="n">
-        <v>0.3498240999999922</v>
+        <v>0.3970567000000074</v>
       </c>
     </row>
     <row r="129">
@@ -6353,7 +6329,7 @@
         <v>53.43539695172467</v>
       </c>
       <c r="X129" t="n">
-        <v>0.2110368999999963</v>
+        <v>0.2289054999999962</v>
       </c>
     </row>
     <row r="130">
@@ -6394,7 +6370,7 @@
         <v>0.7759910627655574</v>
       </c>
       <c r="N130" t="n">
-        <v>0.2187921999999958</v>
+        <v>0.2743179999999938</v>
       </c>
       <c r="O130" t="n">
         <v>8.105205003386365</v>
@@ -6421,7 +6397,7 @@
         <v>40.19682577529397</v>
       </c>
       <c r="X130" t="n">
-        <v>0.3208572000000061</v>
+        <v>0.4039003000000037</v>
       </c>
     </row>
     <row r="131">
@@ -6462,7 +6438,7 @@
         <v>0.569229075708252</v>
       </c>
       <c r="N131" t="n">
-        <v>0.3476074000000011</v>
+        <v>0.4187319999999772</v>
       </c>
     </row>
     <row r="132">
@@ -6540,7 +6516,7 @@
         <v>31.47988333200948</v>
       </c>
       <c r="X134" t="n">
-        <v>0.1267651999999941</v>
+        <v>0.1466350999999975</v>
       </c>
     </row>
     <row r="135">
@@ -6581,7 +6557,7 @@
         <v>0.66177104046478</v>
       </c>
       <c r="N135" t="n">
-        <v>0.2115881000000002</v>
+        <v>0.2657497000000149</v>
       </c>
       <c r="O135" t="n">
         <v>3.510807356990619</v>
@@ -6605,7 +6581,7 @@
         <v>58.56807053357409</v>
       </c>
       <c r="X135" t="n">
-        <v>0.8938612999999975</v>
+        <v>0.9814882000000011</v>
       </c>
     </row>
     <row r="136">
@@ -6646,7 +6622,7 @@
         <v>0.5582792116201171</v>
       </c>
       <c r="N136" t="n">
-        <v>0.223250500000006</v>
+        <v>0.2991735000000233</v>
       </c>
       <c r="O136" t="n">
         <v>11.51789739635981</v>
@@ -6673,7 +6649,7 @@
         <v>45.39224590383571</v>
       </c>
       <c r="X136" t="n">
-        <v>0.1422467000000012</v>
+        <v>0.1578278000000068</v>
       </c>
     </row>
     <row r="137">
@@ -6748,7 +6724,7 @@
         <v>0.6139147613972666</v>
       </c>
       <c r="N139" t="n">
-        <v>0.2002489999999995</v>
+        <v>0.2398923999999738</v>
       </c>
       <c r="O139" t="n">
         <v>8.432087112100337</v>
@@ -6775,7 +6751,7 @@
         <v>41.42690979209499</v>
       </c>
       <c r="X139" t="n">
-        <v>0.1818367000000052</v>
+        <v>0.1620436999999981</v>
       </c>
     </row>
     <row r="140">
@@ -6813,7 +6789,7 @@
         <v>55.42043637027763</v>
       </c>
       <c r="X140" t="n">
-        <v>0.4077436999999975</v>
+        <v>0.4915005000000008</v>
       </c>
     </row>
     <row r="141">
@@ -6854,7 +6830,7 @@
         <v>0.6729219362534257</v>
       </c>
       <c r="N141" t="n">
-        <v>0.2340161000000052</v>
+        <v>0.2888025000000027</v>
       </c>
       <c r="O141" t="n">
         <v>11.87508252603232</v>
@@ -6881,7 +6857,7 @@
         <v>52.1155866369736</v>
       </c>
       <c r="X141" t="n">
-        <v>0.2701873999999975</v>
+        <v>0.2911377000000073</v>
       </c>
     </row>
     <row r="142">
@@ -6942,7 +6918,7 @@
         <v>54.36371412701669</v>
       </c>
       <c r="X143" t="n">
-        <v>0.1264284999999887</v>
+        <v>0.1255095999999867</v>
       </c>
     </row>
     <row r="144">
@@ -7000,7 +6976,7 @@
         <v>0.8558606885423212</v>
       </c>
       <c r="N145" t="n">
-        <v>0.2446707000000004</v>
+        <v>0.2936356999999816</v>
       </c>
     </row>
     <row r="146">
@@ -7092,7 +7068,7 @@
         <v>0.7960451662319317</v>
       </c>
       <c r="N149" t="n">
-        <v>0.2499687999999907</v>
+        <v>0.3059594000000061</v>
       </c>
       <c r="O149" t="n">
         <v>12.91273953453267</v>
@@ -7119,7 +7095,7 @@
         <v>53.81741578465426</v>
       </c>
       <c r="X149" t="n">
-        <v>0.1546981000000045</v>
+        <v>0.1592491000000109</v>
       </c>
     </row>
     <row r="150">
@@ -7160,7 +7136,7 @@
         <v>0.6054464091559779</v>
       </c>
       <c r="N150" t="n">
-        <v>0.3256942000000009</v>
+        <v>0.3847477999999853</v>
       </c>
       <c r="O150" t="n">
         <v>6.277237197854125</v>
@@ -7187,7 +7163,7 @@
         <v>56.18642606325272</v>
       </c>
       <c r="X150" t="n">
-        <v>0.5682992000000127</v>
+        <v>0.6561231999999961</v>
       </c>
     </row>
     <row r="151">
@@ -7228,7 +7204,7 @@
         <v>0.6297107645357374</v>
       </c>
       <c r="N151" t="n">
-        <v>0.2989881000000025</v>
+        <v>0.3630057999999963</v>
       </c>
       <c r="O151" t="n">
         <v>10.52431731741115</v>
@@ -7255,7 +7231,7 @@
         <v>46.43913516348482</v>
       </c>
       <c r="X151" t="n">
-        <v>0.1880134999999967</v>
+        <v>0.2792574000000059</v>
       </c>
     </row>
     <row r="152">
@@ -7313,7 +7289,7 @@
         <v>0.8416314569403841</v>
       </c>
       <c r="N153" t="n">
-        <v>0.233859900000013</v>
+        <v>0.2832270000000108</v>
       </c>
       <c r="O153" t="n">
         <v>12.85689708840115</v>
@@ -7340,7 +7316,7 @@
         <v>59.79472728984803</v>
       </c>
       <c r="X153" t="n">
-        <v>0.2090498000000025</v>
+        <v>0.2319780999999921</v>
       </c>
     </row>
     <row r="154">
@@ -7381,7 +7357,7 @@
         <v>0.8351023701043093</v>
       </c>
       <c r="N154" t="n">
-        <v>0.2518438000000032</v>
+        <v>0.4303371999999968</v>
       </c>
       <c r="O154" t="n">
         <v>9.247466821858925</v>
@@ -7405,7 +7381,7 @@
         <v>19.96918238391919</v>
       </c>
       <c r="X154" t="n">
-        <v>0.168149200000002</v>
+        <v>0.1716726999999878</v>
       </c>
     </row>
     <row r="155">
@@ -7483,7 +7459,7 @@
         <v>46.82679492343993</v>
       </c>
       <c r="X157" t="n">
-        <v>0.5722248000000008</v>
+        <v>0.6129678000000069</v>
       </c>
     </row>
     <row r="158">
@@ -7524,7 +7500,7 @@
         <v>0.9284176031828719</v>
       </c>
       <c r="N158" t="n">
-        <v>0.2483279999999866</v>
+        <v>0.2895212999999899</v>
       </c>
       <c r="O158" t="n">
         <v>15.74351056565251</v>
@@ -7551,7 +7527,7 @@
         <v>54.79504122342809</v>
       </c>
       <c r="X158" t="n">
-        <v>0.279020100000011</v>
+        <v>0.2802376999999865</v>
       </c>
     </row>
     <row r="159">
@@ -7592,7 +7568,7 @@
         <v>0.5852979171129793</v>
       </c>
       <c r="N159" t="n">
-        <v>0.2550734000000006</v>
+        <v>0.3071322000000123</v>
       </c>
       <c r="O159" t="n">
         <v>11.83865318757962</v>
@@ -7619,7 +7595,7 @@
         <v>40.10056931176479</v>
       </c>
       <c r="X159" t="n">
-        <v>0.2151360000000011</v>
+        <v>0.2301530000000014</v>
       </c>
     </row>
     <row r="160">
@@ -7660,7 +7636,7 @@
         <v>0.6356883051023298</v>
       </c>
       <c r="N160" t="n">
-        <v>0.2419072</v>
+        <v>0.3004935999999816</v>
       </c>
       <c r="O160" t="n">
         <v>8.323443435012083</v>
@@ -7687,7 +7663,7 @@
         <v>51.07639331682878</v>
       </c>
       <c r="X160" t="n">
-        <v>0.8610378000000054</v>
+        <v>0.9245102000000145</v>
       </c>
     </row>
     <row r="161">
@@ -7731,7 +7707,7 @@
         <v>49.04768695223601</v>
       </c>
       <c r="X161" t="n">
-        <v>0.1365375999999969</v>
+        <v>0.1571509999999989</v>
       </c>
     </row>
     <row r="162">
@@ -7823,7 +7799,7 @@
         <v>0.6209933235511053</v>
       </c>
       <c r="N165" t="n">
-        <v>0.3021520000000066</v>
+        <v>0.3727388000000076</v>
       </c>
     </row>
     <row r="166">
@@ -7864,7 +7840,7 @@
         <v>0.9462813758820232</v>
       </c>
       <c r="N166" t="n">
-        <v>0.223590999999999</v>
+        <v>0.2845379999999977</v>
       </c>
       <c r="O166" t="n">
         <v>10.6383309008199</v>
@@ -7891,7 +7867,7 @@
         <v>55.91784341088191</v>
       </c>
       <c r="X166" t="n">
-        <v>0.2850044999999994</v>
+        <v>0.3451438000000167</v>
       </c>
     </row>
     <row r="167">
@@ -7932,7 +7908,7 @@
         <v>0.7603749609117307</v>
       </c>
       <c r="N167" t="n">
-        <v>0.2727837000000051</v>
+        <v>0.3894219000000021</v>
       </c>
       <c r="O167" t="n">
         <v>14.5116895743758</v>
@@ -7959,7 +7935,7 @@
         <v>50.05615155655209</v>
       </c>
       <c r="X167" t="n">
-        <v>0.4066179999999946</v>
+        <v>0.4359570000000019</v>
       </c>
     </row>
     <row r="168">
@@ -8003,7 +7979,7 @@
         <v>47.2215047488217</v>
       </c>
       <c r="X168" t="n">
-        <v>0.1864211999999981</v>
+        <v>0.1991127999999946</v>
       </c>
     </row>
     <row r="169">
@@ -8061,7 +8037,7 @@
         <v>0.7472020181523734</v>
       </c>
       <c r="N170" t="n">
-        <v>0.2941842999999977</v>
+        <v>0.3630362999999761</v>
       </c>
       <c r="O170" t="n">
         <v>5.478396406713053</v>
@@ -8088,7 +8064,7 @@
         <v>53.52217043616918</v>
       </c>
       <c r="X170" t="n">
-        <v>1.244551900000005</v>
+        <v>1.453104999999994</v>
       </c>
     </row>
     <row r="171">
@@ -8132,7 +8108,7 @@
         <v>44.46932984274122</v>
       </c>
       <c r="X171" t="n">
-        <v>0.3365415999999897</v>
+        <v>0.4729230000000086</v>
       </c>
     </row>
     <row r="172">
@@ -8207,7 +8183,7 @@
         <v>0.7778893114193726</v>
       </c>
       <c r="N174" t="n">
-        <v>0.1931021999999984</v>
+        <v>0.2659820000000082</v>
       </c>
       <c r="O174" t="n">
         <v>7.33544605418831</v>
@@ -8234,7 +8210,7 @@
         <v>45.91439382765128</v>
       </c>
       <c r="X174" t="n">
-        <v>0.1354879000000011</v>
+        <v>0.1469196000000181</v>
       </c>
     </row>
     <row r="175">
@@ -8275,7 +8251,7 @@
         <v>0.7129290938553247</v>
       </c>
       <c r="N175" t="n">
-        <v>0.1650551999999976</v>
+        <v>0.2517746000000045</v>
       </c>
       <c r="O175" t="n">
         <v>7.600006853986591</v>
@@ -8302,7 +8278,7 @@
         <v>45.7235754559498</v>
       </c>
       <c r="X175" t="n">
-        <v>0.1518104999999963</v>
+        <v>0.1610359000000017</v>
       </c>
     </row>
     <row r="176">
@@ -8343,7 +8319,7 @@
         <v>0.8156080528736385</v>
       </c>
       <c r="N176" t="n">
-        <v>0.1973784000000052</v>
+        <v>0.2522821000000022</v>
       </c>
       <c r="O176" t="n">
         <v>12.39329015034472</v>
@@ -8370,7 +8346,7 @@
         <v>15.89391891279195</v>
       </c>
       <c r="X176" t="n">
-        <v>0.2743922000000083</v>
+        <v>0.3014113999999779</v>
       </c>
     </row>
     <row r="177">
@@ -8414,7 +8390,7 @@
         <v>49.87619890382092</v>
       </c>
       <c r="X177" t="n">
-        <v>0.16343719999999</v>
+        <v>0.1746709999999894</v>
       </c>
     </row>
     <row r="178">
@@ -8458,7 +8434,7 @@
         <v>59.1777193867224</v>
       </c>
       <c r="X178" t="n">
-        <v>0.2764971000000003</v>
+        <v>0.2832932999999969</v>
       </c>
     </row>
     <row r="179">
@@ -8499,7 +8475,7 @@
         <v>0.7048534295841888</v>
       </c>
       <c r="N179" t="n">
-        <v>0.2497314999999958</v>
+        <v>0.4488877000000002</v>
       </c>
       <c r="O179" t="n">
         <v>6.689709649957851</v>
@@ -8526,7 +8502,7 @@
         <v>52.44440852385327</v>
       </c>
       <c r="X179" t="n">
-        <v>0.2403716999999972</v>
+        <v>0.224452499999984</v>
       </c>
     </row>
     <row r="180">
@@ -8567,7 +8543,7 @@
         <v>0.5422282935131407</v>
       </c>
       <c r="N180" t="n">
-        <v>0.4797444000000013</v>
+        <v>0.5782371999999896</v>
       </c>
     </row>
     <row r="181">
@@ -8608,7 +8584,7 @@
         <v>0.6283519641922324</v>
       </c>
       <c r="N181" t="n">
-        <v>0.2203750999999983</v>
+        <v>0.2718224000000191</v>
       </c>
     </row>
     <row r="182">
@@ -8649,7 +8625,7 @@
         <v>0.814099281542769</v>
       </c>
       <c r="N182" t="n">
-        <v>0.2944627999999909</v>
+        <v>0.2311184000000139</v>
       </c>
       <c r="O182" t="n">
         <v>13.74362510448655</v>
@@ -8676,7 +8652,7 @@
         <v>35.02838061829215</v>
       </c>
       <c r="X182" t="n">
-        <v>0.420807300000007</v>
+        <v>0.4436105999999995</v>
       </c>
     </row>
     <row r="183">
@@ -8734,7 +8710,7 @@
         <v>0.572575338807719</v>
       </c>
       <c r="N184" t="n">
-        <v>0.2021426000000019</v>
+        <v>0.2805483999999865</v>
       </c>
     </row>
     <row r="185">
@@ -8778,7 +8754,7 @@
         <v>40.08249783381137</v>
       </c>
       <c r="X185" t="n">
-        <v>0.2176160000000067</v>
+        <v>0.2368785000000457</v>
       </c>
     </row>
     <row r="186">
@@ -8822,7 +8798,7 @@
         <v>31.25903791033352</v>
       </c>
       <c r="X186" t="n">
-        <v>0.1936160999999998</v>
+        <v>0.1970769000000132</v>
       </c>
     </row>
     <row r="187">
@@ -8863,7 +8839,7 @@
         <v>0.6090177363515266</v>
       </c>
       <c r="N187" t="n">
-        <v>1.073143200000004</v>
+        <v>1.126889100000028</v>
       </c>
       <c r="O187" t="n">
         <v>16.02846480082625</v>
@@ -8890,7 +8866,7 @@
         <v>56.29129486229522</v>
       </c>
       <c r="X187" t="n">
-        <v>0.197662600000001</v>
+        <v>0.1846082999999794</v>
       </c>
     </row>
     <row r="188">
@@ -8931,7 +8907,7 @@
         <v>0.7505504670917696</v>
       </c>
       <c r="N188" t="n">
-        <v>0.2366772000000026</v>
+        <v>0.2891850999999974</v>
       </c>
       <c r="O188" t="n">
         <v>12.61238131548211</v>
@@ -8958,7 +8934,7 @@
         <v>34.77992114627597</v>
       </c>
       <c r="X188" t="n">
-        <v>0.1725732999999963</v>
+        <v>0.1756368000000066</v>
       </c>
     </row>
     <row r="189">
@@ -9002,7 +8978,7 @@
         <v>51.7118211970843</v>
       </c>
       <c r="X189" t="n">
-        <v>0.4481174999999951</v>
+        <v>0.5086716999999794</v>
       </c>
     </row>
     <row r="190">
@@ -9043,7 +9019,7 @@
         <v>0.6863154554326605</v>
       </c>
       <c r="N190" t="n">
-        <v>0.2281285999999909</v>
+        <v>0.2912193999999886</v>
       </c>
     </row>
     <row r="191">
@@ -9084,7 +9060,7 @@
         <v>0.6236299671445056</v>
       </c>
       <c r="N191" t="n">
-        <v>0.2790266000000088</v>
+        <v>0.3189706000000001</v>
       </c>
       <c r="O191" t="n">
         <v>9.625332320788159</v>
@@ -9108,7 +9084,7 @@
         <v>16.75456998731744</v>
       </c>
       <c r="X191" t="n">
-        <v>0.227103800000009</v>
+        <v>0.2628634000000147</v>
       </c>
     </row>
     <row r="192">
@@ -9166,7 +9142,7 @@
         <v>0.6519022263066028</v>
       </c>
       <c r="N193" t="n">
-        <v>0.7424099999999783</v>
+        <v>0.9212594999999624</v>
       </c>
       <c r="O193" t="n">
         <v>5.216687189586056</v>
@@ -9193,7 +9169,7 @@
         <v>58.08918250403576</v>
       </c>
       <c r="X193" t="n">
-        <v>0.1727608999999859</v>
+        <v>0.2029987000000233</v>
       </c>
     </row>
     <row r="194">
@@ -9234,7 +9210,7 @@
         <v>0.6991461269116794</v>
       </c>
       <c r="N194" t="n">
-        <v>0.2265387000000203</v>
+        <v>0.2897601999999893</v>
       </c>
       <c r="O194" t="n">
         <v>13.20762461494212</v>
@@ -9261,7 +9237,7 @@
         <v>35.86478916565011</v>
       </c>
       <c r="X194" t="n">
-        <v>0.3698165000000131</v>
+        <v>0.3922673000000145</v>
       </c>
     </row>
     <row r="195">
@@ -9302,7 +9278,7 @@
         <v>0.6734162523265559</v>
       </c>
       <c r="N195" t="n">
-        <v>0.5423533999999961</v>
+        <v>0.781216900000004</v>
       </c>
       <c r="O195" t="n">
         <v>6.4533509661202</v>
@@ -9329,7 +9305,7 @@
         <v>44.44825355494731</v>
       </c>
       <c r="X195" t="n">
-        <v>0.3437007999999935</v>
+        <v>0.3883758000000057</v>
       </c>
     </row>
     <row r="196">
@@ -9390,7 +9366,7 @@
         <v>31.99759926785424</v>
       </c>
       <c r="X197" t="n">
-        <v>0.1370538999999837</v>
+        <v>0.1544418999999948</v>
       </c>
     </row>
     <row r="198">
@@ -9431,7 +9407,7 @@
         <v>0.6447031392336856</v>
       </c>
       <c r="N198" t="n">
-        <v>0.7522013999999899</v>
+        <v>0.8941963000000328</v>
       </c>
     </row>
     <row r="199">
@@ -9472,7 +9448,7 @@
         <v>0.5760591443043799</v>
       </c>
       <c r="N199" t="n">
-        <v>1.0070044</v>
+        <v>1.109849999999994</v>
       </c>
       <c r="O199" t="n">
         <v>11.15054723768442</v>
@@ -9499,7 +9475,7 @@
         <v>52.23679605371535</v>
       </c>
       <c r="X199" t="n">
-        <v>0.1983331999999791</v>
+        <v>0.2250229999999647</v>
       </c>
     </row>
     <row r="200">
@@ -9543,7 +9519,7 @@
         <v>41.06823991440251</v>
       </c>
       <c r="X200" t="n">
-        <v>0.2246667000000002</v>
+        <v>0.2708096000000069</v>
       </c>
     </row>
     <row r="201">
@@ -9587,7 +9563,7 @@
         <v>41.10933814146318</v>
       </c>
       <c r="X201" t="n">
-        <v>0.3949431000000061</v>
+        <v>0.4713590000000067</v>
       </c>
     </row>
     <row r="202">
@@ -9628,7 +9604,7 @@
         <v>0.782415012994204</v>
       </c>
       <c r="N202" t="n">
-        <v>0.2854703999999799</v>
+        <v>0.3690368000000035</v>
       </c>
     </row>
     <row r="203">
@@ -9686,7 +9662,7 @@
         <v>0.503557118560361</v>
       </c>
       <c r="N204" t="n">
-        <v>0.6115700000000004</v>
+        <v>0.7463981000000217</v>
       </c>
     </row>
     <row r="205">
@@ -9727,7 +9703,7 @@
         <v>0.5438033381585889</v>
       </c>
       <c r="N205" t="n">
-        <v>0.3127451999999948</v>
+        <v>0.3920678999999723</v>
       </c>
       <c r="O205" t="n">
         <v>8.275524047001236</v>
@@ -9754,7 +9730,7 @@
         <v>44.28155390322712</v>
       </c>
       <c r="X205" t="n">
-        <v>0.3838481999999885</v>
+        <v>0.4608219000000418</v>
       </c>
     </row>
     <row r="206">
@@ -9795,7 +9771,7 @@
         <v>0.7207876541638537</v>
       </c>
       <c r="N206" t="n">
-        <v>0.1757536000000073</v>
+        <v>0.234814799999981</v>
       </c>
       <c r="O206" t="n">
         <v>12.93941500037211</v>
@@ -9822,7 +9798,7 @@
         <v>38.2256305804159</v>
       </c>
       <c r="X206" t="n">
-        <v>0.5621460000000127</v>
+        <v>0.6048597999999856</v>
       </c>
     </row>
     <row r="207">
@@ -9863,7 +9839,7 @@
         <v>0.7614454848345248</v>
       </c>
       <c r="N207" t="n">
-        <v>0.2574338000000012</v>
+        <v>0.3686116000000084</v>
       </c>
       <c r="O207" t="n">
         <v>17.86380172625017</v>
@@ -9890,7 +9866,7 @@
         <v>32.14037721232523</v>
       </c>
       <c r="X207" t="n">
-        <v>0.2783975000000112</v>
+        <v>0.327067100000022</v>
       </c>
     </row>
     <row r="208">
@@ -9931,7 +9907,7 @@
         <v>0.7850982936704513</v>
       </c>
       <c r="N208" t="n">
-        <v>0.2323817999999847</v>
+        <v>0.3092391999999791</v>
       </c>
       <c r="O208" t="n">
         <v>8.685343267640484</v>
@@ -9958,7 +9934,7 @@
         <v>41.45273931922247</v>
       </c>
       <c r="X208" t="n">
-        <v>0.237308999999982</v>
+        <v>0.3053113999999937</v>
       </c>
     </row>
     <row r="209">
@@ -9999,7 +9975,7 @@
         <v>0.5801759708679762</v>
       </c>
       <c r="N209" t="n">
-        <v>0.3083665999999994</v>
+        <v>0.4019395999999915</v>
       </c>
       <c r="O209" t="n">
         <v>7.713577086904683</v>
@@ -10026,7 +10002,7 @@
         <v>52.45552571319683</v>
       </c>
       <c r="X209" t="n">
-        <v>0.8269641999999919</v>
+        <v>0.9513299999999845</v>
       </c>
     </row>
     <row r="210">
@@ -10067,7 +10043,7 @@
         <v>0.6433097552103763</v>
       </c>
       <c r="N210" t="n">
-        <v>0.711685000000017</v>
+        <v>0.86389029999998</v>
       </c>
       <c r="O210" t="n">
         <v>5.789287178664564</v>
@@ -10094,7 +10070,7 @@
         <v>36.24008230675787</v>
       </c>
       <c r="X210" t="n">
-        <v>0.1104185999999743</v>
+        <v>0.1210042999999814</v>
       </c>
     </row>
     <row r="211">
@@ -10135,7 +10111,7 @@
         <v>0.7077004049317255</v>
       </c>
       <c r="N211" t="n">
-        <v>0.2097167999999954</v>
+        <v>0.3974176999999486</v>
       </c>
       <c r="O211" t="n">
         <v>10.88197860710382</v>
@@ -10162,7 +10138,7 @@
         <v>55.39376284974031</v>
       </c>
       <c r="X211" t="n">
-        <v>0.3149277999999924</v>
+        <v>0.3746679000000199</v>
       </c>
     </row>
     <row r="212">
@@ -10257,7 +10233,7 @@
         <v>56.55405614171275</v>
       </c>
       <c r="X215" t="n">
-        <v>0.3519292000000007</v>
+        <v>0.414815400000009</v>
       </c>
     </row>
     <row r="216">
@@ -10298,7 +10274,7 @@
         <v>0.6078827981757445</v>
       </c>
       <c r="N216" t="n">
-        <v>0.2365537999999958</v>
+        <v>0.3144594000000325</v>
       </c>
       <c r="O216" t="n">
         <v>8.853002355128242</v>
@@ -10325,7 +10301,7 @@
         <v>43.54504166427375</v>
       </c>
       <c r="X216" t="n">
-        <v>0.1007622999999853</v>
+        <v>0.1118285000000014</v>
       </c>
     </row>
     <row r="217">
@@ -10366,7 +10342,7 @@
         <v>0.7183214183995025</v>
       </c>
       <c r="N217" t="n">
-        <v>0.1802990999999849</v>
+        <v>0.2364819999999668</v>
       </c>
       <c r="O217" t="n">
         <v>3.46310111957435</v>
@@ -10390,7 +10366,7 @@
         <v>50.46704197121431</v>
       </c>
       <c r="X217" t="n">
-        <v>1.209082300000006</v>
+        <v>1.407641000000012</v>
       </c>
     </row>
     <row r="218">
@@ -10434,7 +10410,7 @@
         <v>52.53270519824861</v>
       </c>
       <c r="X218" t="n">
-        <v>0.2274685000000147</v>
+        <v>0.2803706000000261</v>
       </c>
     </row>
     <row r="219">
@@ -10478,7 +10454,7 @@
         <v>41.11439435217051</v>
       </c>
       <c r="X219" t="n">
-        <v>0.1881223999999975</v>
+        <v>0.2132490999999845</v>
       </c>
     </row>
     <row r="220">
@@ -10604,7 +10580,7 @@
         <v>0.7480150249470665</v>
       </c>
       <c r="N225" t="n">
-        <v>0.3526664000000039</v>
+        <v>0.4479420000000118</v>
       </c>
       <c r="O225" t="n">
         <v>11.32248837693816</v>
@@ -10631,7 +10607,7 @@
         <v>54.81975454632305</v>
       </c>
       <c r="X225" t="n">
-        <v>0.4211430000000007</v>
+        <v>0.4586714000000143</v>
       </c>
     </row>
     <row r="226">
@@ -10672,7 +10648,7 @@
         <v>0.7954285075936763</v>
       </c>
       <c r="N226" t="n">
-        <v>0.1762765999999942</v>
+        <v>0.2375208000000271</v>
       </c>
       <c r="O226" t="n">
         <v>12.00675460680065</v>
@@ -10699,7 +10675,7 @@
         <v>22.1569853107398</v>
       </c>
       <c r="X226" t="n">
-        <v>0.2155785999999864</v>
+        <v>0.2804884999999899</v>
       </c>
     </row>
     <row r="227">
@@ -10743,7 +10719,7 @@
         <v>50.64256292884659</v>
       </c>
       <c r="X227" t="n">
-        <v>0.2217540000000042</v>
+        <v>0.3056950999999799</v>
       </c>
     </row>
     <row r="228">
@@ -10784,7 +10760,7 @@
         <v>0.8316444744474988</v>
       </c>
       <c r="N228" t="n">
-        <v>0.2689225999999962</v>
+        <v>0.3355225999999902</v>
       </c>
       <c r="O228" t="n">
         <v>14.14308152436669</v>
@@ -10811,7 +10787,7 @@
         <v>44.06370669845751</v>
       </c>
       <c r="X228" t="n">
-        <v>0.196380199999993</v>
+        <v>0.2130937999999674</v>
       </c>
     </row>
     <row r="229">
@@ -10855,7 +10831,7 @@
         <v>41.55535421956677</v>
       </c>
       <c r="X229" t="n">
-        <v>0.1394329000000027</v>
+        <v>0.1556381999999985</v>
       </c>
     </row>
     <row r="230">
@@ -10913,7 +10889,7 @@
         <v>0.5299909355820348</v>
       </c>
       <c r="N231" t="n">
-        <v>0.1673040999999955</v>
+        <v>0.2266840999999999</v>
       </c>
       <c r="O231" t="n">
         <v>3.807943758671646</v>
@@ -10940,7 +10916,7 @@
         <v>31.70931821363479</v>
       </c>
       <c r="X231" t="n">
-        <v>0.09309220000000096</v>
+        <v>0.1029376000000184</v>
       </c>
     </row>
     <row r="232">
@@ -10998,7 +10974,7 @@
         <v>0.7456745576053355</v>
       </c>
       <c r="N233" t="n">
-        <v>0.1903882999999951</v>
+        <v>0.2615996999999766</v>
       </c>
       <c r="O233" t="n">
         <v>13.58829959015713</v>
@@ -11025,7 +11001,7 @@
         <v>53.45936777484468</v>
       </c>
       <c r="X233" t="n">
-        <v>0.216099000000014</v>
+        <v>0.2347188999999616</v>
       </c>
     </row>
     <row r="234">
@@ -11066,7 +11042,7 @@
         <v>0.6551296709362725</v>
       </c>
       <c r="N234" t="n">
-        <v>0.2567921000000126</v>
+        <v>0.4444072999999662</v>
       </c>
     </row>
     <row r="235">
@@ -11107,7 +11083,7 @@
         <v>0.7544759929895687</v>
       </c>
       <c r="N235" t="n">
-        <v>0.2588655999999787</v>
+        <v>0.3506279000000063</v>
       </c>
     </row>
     <row r="236">
@@ -11165,7 +11141,7 @@
         <v>0.6973238519931545</v>
       </c>
       <c r="N237" t="n">
-        <v>0.2575888000000077</v>
+        <v>0.3169968000000267</v>
       </c>
       <c r="O237" t="n">
         <v>7.066212521311115</v>
@@ -11192,7 +11168,7 @@
         <v>48.660419729311</v>
       </c>
       <c r="X237" t="n">
-        <v>0.1793061000000193</v>
+        <v>0.1994896999999582</v>
       </c>
     </row>
     <row r="238">
@@ -11230,7 +11206,7 @@
         <v>47.45897914785075</v>
       </c>
       <c r="X238" t="n">
-        <v>0.2268191000000002</v>
+        <v>0.2569255999999882</v>
       </c>
     </row>
     <row r="239">
@@ -11271,7 +11247,7 @@
         <v>0.5198072735514186</v>
       </c>
       <c r="N239" t="n">
-        <v>0.2402395999999953</v>
+        <v>0.2940649999999891</v>
       </c>
       <c r="O239" t="n">
         <v>11.77171525468184</v>
@@ -11298,7 +11274,7 @@
         <v>46.30647699894831</v>
       </c>
       <c r="X239" t="n">
-        <v>0.1872303000000102</v>
+        <v>0.2056920999999647</v>
       </c>
     </row>
     <row r="240">
@@ -11356,7 +11332,7 @@
         <v>0.7729427953021996</v>
       </c>
       <c r="N241" t="n">
-        <v>0.4606014999999957</v>
+        <v>0.5724068000000102</v>
       </c>
       <c r="O241" t="n">
         <v>16.88767985816003</v>
@@ -11383,7 +11359,7 @@
         <v>58.73543187174175</v>
       </c>
       <c r="X241" t="n">
-        <v>0.2615447000000017</v>
+        <v>0.3032224999999471</v>
       </c>
     </row>
     <row r="242">
@@ -11424,7 +11400,7 @@
         <v>0.5135217450418931</v>
       </c>
       <c r="N242" t="n">
-        <v>0.2176645000000121</v>
+        <v>0.2731271000000106</v>
       </c>
       <c r="O242" t="n">
         <v>8.642245936020171</v>
@@ -11451,7 +11427,7 @@
         <v>10.51377780172834</v>
       </c>
       <c r="X242" t="n">
-        <v>0.1436881000000199</v>
+        <v>0.1549317999999857</v>
       </c>
     </row>
     <row r="243">
@@ -11495,7 +11471,7 @@
         <v>44.91580328599429</v>
       </c>
       <c r="X243" t="n">
-        <v>0.7924983999999995</v>
+        <v>0.9358550000000037</v>
       </c>
     </row>
     <row r="244">
@@ -11553,7 +11529,7 @@
         <v>0.5222236691638125</v>
       </c>
       <c r="N245" t="n">
-        <v>0.2589257999999859</v>
+        <v>0.3167104999999992</v>
       </c>
       <c r="O245" t="n">
         <v>10.9526133776974</v>
@@ -11580,7 +11556,7 @@
         <v>50.77072992585659</v>
       </c>
       <c r="X245" t="n">
-        <v>0.2342706000000021</v>
+        <v>0.2488148999999567</v>
       </c>
     </row>
     <row r="246">
@@ -11621,7 +11597,7 @@
         <v>0.5999657106355182</v>
       </c>
       <c r="N246" t="n">
-        <v>0.1676319000000035</v>
+        <v>0.3442885000000047</v>
       </c>
       <c r="O246" t="n">
         <v>5.613571937167778</v>
@@ -11648,7 +11624,7 @@
         <v>51.84465779013937</v>
       </c>
       <c r="X246" t="n">
-        <v>0.4505030999999917</v>
+        <v>0.5346576999999684</v>
       </c>
     </row>
     <row r="247">
@@ -11689,7 +11665,7 @@
         <v>0.7860287964581961</v>
       </c>
       <c r="N247" t="n">
-        <v>0.2276752999999871</v>
+        <v>0.300563899999986</v>
       </c>
       <c r="O247" t="n">
         <v>6.585357387244891</v>
@@ -11716,7 +11692,7 @@
         <v>35.04845187343415</v>
       </c>
       <c r="X247" t="n">
-        <v>0.1525938999999994</v>
+        <v>0.1680332999999905</v>
       </c>
     </row>
     <row r="248">
@@ -11757,7 +11733,7 @@
         <v>0.7386735311150414</v>
       </c>
       <c r="N248" t="n">
-        <v>0.2202298999999925</v>
+        <v>0.27131270000001</v>
       </c>
       <c r="O248" t="n">
         <v>7.159696601410431</v>
@@ -11784,7 +11760,7 @@
         <v>32.09591535847187</v>
       </c>
       <c r="X248" t="n">
-        <v>0.4033472000000131</v>
+        <v>0.4426563999999757</v>
       </c>
     </row>
     <row r="249">
@@ -11825,7 +11801,7 @@
         <v>0.7542459245456868</v>
       </c>
       <c r="N249" t="n">
-        <v>0.2419083999999998</v>
+        <v>0.3013145000000463</v>
       </c>
       <c r="O249" t="n">
         <v>10.38013409313423</v>
@@ -11852,7 +11828,7 @@
         <v>55.83004897783917</v>
       </c>
       <c r="X249" t="n">
-        <v>0.1590121000000124</v>
+        <v>0.1801580999999715</v>
       </c>
     </row>
     <row r="250">
@@ -11893,7 +11869,7 @@
         <v>0.8527506665673604</v>
       </c>
       <c r="N250" t="n">
-        <v>0.215688799999981</v>
+        <v>0.2726490000000013</v>
       </c>
       <c r="O250" t="n">
         <v>15.83351800973342</v>
@@ -11920,7 +11896,7 @@
         <v>58.44281607161616</v>
       </c>
       <c r="X250" t="n">
-        <v>0.422327700000011</v>
+        <v>0.5293929000000048</v>
       </c>
     </row>
     <row r="251">
@@ -11961,7 +11937,7 @@
         <v>0.5849756032409672</v>
       </c>
       <c r="N251" t="n">
-        <v>0.2235894000000087</v>
+        <v>0.2795345999999768</v>
       </c>
       <c r="O251" t="n">
         <v>7.861869118386146</v>
@@ -11988,7 +11964,7 @@
         <v>57.68850573345622</v>
       </c>
       <c r="X251" t="n">
-        <v>0.2859775000000013</v>
+        <v>0.3286970999999994</v>
       </c>
     </row>
     <row r="252">
@@ -12029,7 +12005,7 @@
         <v>0.624117025596622</v>
       </c>
       <c r="N252" t="n">
-        <v>0.5274292000000003</v>
+        <v>0.7009654000000296</v>
       </c>
     </row>
     <row r="253">
@@ -12070,7 +12046,7 @@
         <v>0.6419686597652164</v>
       </c>
       <c r="N253" t="n">
-        <v>0.2000716999999952</v>
+        <v>0.2572674000000461</v>
       </c>
     </row>
     <row r="254">
@@ -12114,7 +12090,7 @@
         <v>55.01923652826514</v>
       </c>
       <c r="X254" t="n">
-        <v>0.1700917000000004</v>
+        <v>0.197306900000001</v>
       </c>
     </row>
     <row r="255">
@@ -12155,7 +12131,7 @@
         <v>0.6581219376323464</v>
       </c>
       <c r="N255" t="n">
-        <v>0.7213694000000146</v>
+        <v>0.8964653999999541</v>
       </c>
       <c r="O255" t="n">
         <v>7.689003362713681</v>
@@ -12182,7 +12158,7 @@
         <v>32.56390702090044</v>
       </c>
       <c r="X255" t="n">
-        <v>0.342940700000014</v>
+        <v>0.4275357999999869</v>
       </c>
     </row>
     <row r="256">
@@ -12223,7 +12199,7 @@
         <v>0.705920964233881</v>
       </c>
       <c r="N256" t="n">
-        <v>0.2392604000000063</v>
+        <v>0.2995710999999801</v>
       </c>
       <c r="O256" t="n">
         <v>7.794572257281294</v>
@@ -12250,7 +12226,7 @@
         <v>35.41513015494758</v>
       </c>
       <c r="X256" t="n">
-        <v>0.1639776000000097</v>
+        <v>0.1765163999999686</v>
       </c>
     </row>
     <row r="257">
@@ -12311,7 +12287,7 @@
         <v>53.83641217865465</v>
       </c>
       <c r="X258" t="n">
-        <v>0.295687700000002</v>
+        <v>0.3374512999999979</v>
       </c>
     </row>
     <row r="259">
@@ -12352,7 +12328,7 @@
         <v>0.7048733607010829</v>
       </c>
       <c r="N259" t="n">
-        <v>0.2786648000000014</v>
+        <v>0.3314116999999897</v>
       </c>
     </row>
     <row r="260">
@@ -12393,7 +12369,7 @@
         <v>0.667571086807434</v>
       </c>
       <c r="N260" t="n">
-        <v>0.2303765000000055</v>
+        <v>0.2762708000000202</v>
       </c>
     </row>
     <row r="261">
@@ -12434,7 +12410,7 @@
         <v>0.7847440459549182</v>
       </c>
       <c r="N261" t="n">
-        <v>0.2665283000000045</v>
+        <v>0.301047600000004</v>
       </c>
     </row>
     <row r="262">
@@ -12475,7 +12451,7 @@
         <v>0.6182734847249527</v>
       </c>
       <c r="N262" t="n">
-        <v>0.2989342000000192</v>
+        <v>0.3153757000000041</v>
       </c>
     </row>
     <row r="263">
@@ -12550,7 +12526,7 @@
         <v>0.749132990600455</v>
       </c>
       <c r="N265" t="n">
-        <v>0.2106749999999806</v>
+        <v>0.2726312000000348</v>
       </c>
       <c r="O265" t="n">
         <v>10.63804465150137</v>
@@ -12577,7 +12553,7 @@
         <v>50.78198565492403</v>
       </c>
       <c r="X265" t="n">
-        <v>0.2886636000000067</v>
+        <v>0.3138074999999958</v>
       </c>
     </row>
     <row r="266">
@@ -12618,7 +12594,7 @@
         <v>0.7926910889900537</v>
       </c>
       <c r="N266" t="n">
-        <v>0.2413720000000126</v>
+        <v>0.2928449999999998</v>
       </c>
     </row>
     <row r="267">
@@ -12676,7 +12652,7 @@
         <v>0.8893562571831392</v>
       </c>
       <c r="N268" t="n">
-        <v>0.2225545999999952</v>
+        <v>0.2750452999999879</v>
       </c>
     </row>
     <row r="269">
@@ -12734,7 +12710,7 @@
         <v>0.780535590502386</v>
       </c>
       <c r="N270" t="n">
-        <v>0.3831126999999981</v>
+        <v>0.4584494000000063</v>
       </c>
     </row>
     <row r="271">
@@ -12775,7 +12751,7 @@
         <v>0.7476205642373706</v>
       </c>
       <c r="N271" t="n">
-        <v>0.2144002999999941</v>
+        <v>0.2948794000000134</v>
       </c>
     </row>
     <row r="272">
@@ -12816,7 +12792,7 @@
         <v>0.5933136613025117</v>
       </c>
       <c r="N272" t="n">
-        <v>0.2576523000000179</v>
+        <v>0.3176354999999944</v>
       </c>
     </row>
     <row r="273">
@@ -12857,7 +12833,7 @@
         <v>0.5579226106722425</v>
       </c>
       <c r="N273" t="n">
-        <v>0.2422259999999881</v>
+        <v>0.3658491000000481</v>
       </c>
       <c r="O273" t="n">
         <v>5.265836946360143</v>
@@ -12884,7 +12860,7 @@
         <v>52.1347451406852</v>
       </c>
       <c r="X273" t="n">
-        <v>0.179939399999995</v>
+        <v>0.1952110000000289</v>
       </c>
     </row>
     <row r="274">
@@ -12922,7 +12898,7 @@
         <v>57.05277684659177</v>
       </c>
       <c r="X274" t="n">
-        <v>1.021446700000013</v>
+        <v>1.323904700000014</v>
       </c>
     </row>
     <row r="275">
@@ -12963,7 +12939,7 @@
         <v>0.8582887586803196</v>
       </c>
       <c r="N275" t="n">
-        <v>0.3930436999999927</v>
+        <v>0.4923661000000266</v>
       </c>
       <c r="O275" t="n">
         <v>7.863476849427554</v>
@@ -12990,7 +12966,7 @@
         <v>27.58621225378675</v>
       </c>
       <c r="X275" t="n">
-        <v>0.2236653000000217</v>
+        <v>0.2582126000000358</v>
       </c>
     </row>
     <row r="276">
@@ -13065,7 +13041,7 @@
         <v>0.8031583639784863</v>
       </c>
       <c r="N278" t="n">
-        <v>0.2262257999999804</v>
+        <v>0.2861469000000056</v>
       </c>
       <c r="O278" t="n">
         <v>9.269626487408967</v>
@@ -13092,7 +13068,7 @@
         <v>50.22548555909117</v>
       </c>
       <c r="X278" t="n">
-        <v>0.3569612999999947</v>
+        <v>0.4467332000000397</v>
       </c>
     </row>
     <row r="279">
@@ -13133,7 +13109,7 @@
         <v>0.622932114668151</v>
       </c>
       <c r="N279" t="n">
-        <v>0.2584004999999934</v>
+        <v>0.3217149999999833</v>
       </c>
       <c r="O279" t="n">
         <v>12.5483241184886</v>
@@ -13160,7 +13136,7 @@
         <v>11.66727437125792</v>
       </c>
       <c r="X279" t="n">
-        <v>0.155706500000008</v>
+        <v>0.1703559999999698</v>
       </c>
     </row>
     <row r="280">
@@ -13221,7 +13197,7 @@
         <v>58.515930590464</v>
       </c>
       <c r="X281" t="n">
-        <v>0.1876345000000015</v>
+        <v>0.2089178999999604</v>
       </c>
     </row>
     <row r="282">
@@ -13262,7 +13238,7 @@
         <v>0.5586334855331648</v>
       </c>
       <c r="N282" t="n">
-        <v>0.3961027999999942</v>
+        <v>0.4984788000000435</v>
       </c>
       <c r="O282" t="n">
         <v>13.04871656190554</v>
@@ -13289,7 +13265,7 @@
         <v>46.39715553091321</v>
       </c>
       <c r="X282" t="n">
-        <v>1.030781399999995</v>
+        <v>1.149377600000037</v>
       </c>
     </row>
     <row r="283">
@@ -13364,7 +13340,7 @@
         <v>0.8297853709879708</v>
       </c>
       <c r="N285" t="n">
-        <v>0.2311594999999897</v>
+        <v>0.2959491999999955</v>
       </c>
       <c r="O285" t="n">
         <v>15.48882826758408</v>
@@ -13391,7 +13367,7 @@
         <v>44.6819014977566</v>
       </c>
       <c r="X285" t="n">
-        <v>0.1809749999999894</v>
+        <v>0.2336058999999864</v>
       </c>
     </row>
     <row r="286">
@@ -13449,7 +13425,7 @@
         <v>0.5194741443694612</v>
       </c>
       <c r="N287" t="n">
-        <v>0.3819063999999912</v>
+        <v>0.4784985000000006</v>
       </c>
       <c r="O287" t="n">
         <v>14.08542813081427</v>
@@ -13476,7 +13452,7 @@
         <v>58.81957177017364</v>
       </c>
       <c r="X287" t="n">
-        <v>0.1849492000000055</v>
+        <v>0.1955277000000137</v>
       </c>
     </row>
     <row r="288">
@@ -13517,7 +13493,7 @@
         <v>0.7974668826670378</v>
       </c>
       <c r="N288" t="n">
-        <v>0.2851280000000145</v>
+        <v>0.3453124000000116</v>
       </c>
     </row>
     <row r="289">
@@ -13558,7 +13534,7 @@
         <v>0.7950150162254952</v>
       </c>
       <c r="N289" t="n">
-        <v>0.245002999999997</v>
+        <v>0.3096918999999616</v>
       </c>
       <c r="O289" t="n">
         <v>15.2665675690923</v>
@@ -13585,7 +13561,7 @@
         <v>42.44265984796442</v>
       </c>
       <c r="X289" t="n">
-        <v>0.158128099999999</v>
+        <v>0.1642779000000019</v>
       </c>
     </row>
     <row r="290">
@@ -13629,7 +13605,7 @@
         <v>46.4404152897402</v>
       </c>
       <c r="X290" t="n">
-        <v>0.4107520000000022</v>
+        <v>0.5272396000000299</v>
       </c>
     </row>
     <row r="291">
@@ -13670,7 +13646,7 @@
         <v>0.7486908851655873</v>
       </c>
       <c r="N291" t="n">
-        <v>0.3027767999999753</v>
+        <v>0.3749334999999974</v>
       </c>
       <c r="O291" t="n">
         <v>12.84654444047575</v>
@@ -13697,7 +13673,7 @@
         <v>57.70163646234255</v>
       </c>
       <c r="X291" t="n">
-        <v>0.4865975000000162</v>
+        <v>0.6320557000000235</v>
       </c>
     </row>
     <row r="292">
@@ -13738,7 +13714,7 @@
         <v>0.8111038024407007</v>
       </c>
       <c r="N292" t="n">
-        <v>0.1536407000000111</v>
+        <v>0.2226089999999772</v>
       </c>
       <c r="O292" t="n">
         <v>4.44372029261366</v>
@@ -13765,7 +13741,7 @@
         <v>59.62019214347447</v>
       </c>
       <c r="X292" t="n">
-        <v>1.620365399999997</v>
+        <v>1.99759320000004</v>
       </c>
     </row>
     <row r="293">
@@ -13806,7 +13782,7 @@
         <v>0.7967663846017742</v>
       </c>
       <c r="N293" t="n">
-        <v>0.1901900999999953</v>
+        <v>0.2596712000000139</v>
       </c>
     </row>
     <row r="294">
@@ -13847,7 +13823,7 @@
         <v>0.5396645747654271</v>
       </c>
       <c r="N294" t="n">
-        <v>0.3738630999999941</v>
+        <v>0.4854535000000055</v>
       </c>
       <c r="O294" t="n">
         <v>3.104462088646399</v>
@@ -13868,7 +13844,7 @@
         <v>58.0197520733285</v>
       </c>
       <c r="X294" t="n">
-        <v>0.7680916000000195</v>
+        <v>0.953669600000012</v>
       </c>
     </row>
     <row r="295">
@@ -13909,7 +13885,7 @@
         <v>0.7582074252020459</v>
       </c>
       <c r="N295" t="n">
-        <v>0.3456687000000045</v>
+        <v>0.4575738999999999</v>
       </c>
       <c r="O295" t="n">
         <v>8.315672261038857</v>
@@ -13936,7 +13912,7 @@
         <v>59.21255483842174</v>
       </c>
       <c r="X295" t="n">
-        <v>0.2679952000000014</v>
+        <v>0.3303591000000097</v>
       </c>
     </row>
     <row r="296">
@@ -13977,7 +13953,7 @@
         <v>0.8660976179885116</v>
       </c>
       <c r="N296" t="n">
-        <v>0.2524107000000129</v>
+        <v>0.3325820999999678</v>
       </c>
       <c r="O296" t="n">
         <v>11.4265202241095</v>
@@ -14004,7 +13980,7 @@
         <v>59.64368308853756</v>
       </c>
       <c r="X296" t="n">
-        <v>0.2774443000000133</v>
+        <v>0.3094332999999665</v>
       </c>
     </row>
     <row r="297">
@@ -14062,7 +14038,7 @@
         <v>0.7302239438641055</v>
       </c>
       <c r="N298" t="n">
-        <v>0.152940099999995</v>
+        <v>0.2245608999999718</v>
       </c>
       <c r="O298" t="n">
         <v>8.31214379105888</v>
@@ -14089,7 +14065,7 @@
         <v>51.75104565055506</v>
       </c>
       <c r="X298" t="n">
-        <v>0.2452557999999954</v>
+        <v>0.3191797000000065</v>
       </c>
     </row>
     <row r="299">
@@ -14164,7 +14140,7 @@
         <v>0.5764296229561046</v>
       </c>
       <c r="N301" t="n">
-        <v>0.1611298999999917</v>
+        <v>0.2261900999999966</v>
       </c>
       <c r="O301" t="n">
         <v>7.77308427608896</v>
@@ -14191,7 +14167,7 @@
         <v>57.45608137614971</v>
       </c>
       <c r="X301" t="n">
-        <v>0.1504979000000048</v>
+        <v>0.2465020999999865</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added legend for the html files
</commit_message>
<xml_diff>
--- a/webapp/data.xlsx
+++ b/webapp/data.xlsx
@@ -513,7 +513,7 @@
         <v>0.6862360802795323</v>
       </c>
       <c r="N2" t="n">
-        <v>0.5078755999999984</v>
+        <v>1.603566499999999</v>
       </c>
       <c r="O2" t="n">
         <v>7.082991651314155</v>
@@ -540,7 +540,7 @@
         <v>59.77815053634509</v>
       </c>
       <c r="X2" t="n">
-        <v>0.2486348000000014</v>
+        <v>0.2475695000000044</v>
       </c>
     </row>
     <row r="3">
@@ -560,10 +560,10 @@
         <v>2375</v>
       </c>
       <c r="F3" t="n">
-        <v>10.52886351203547</v>
+        <v>11.62283920279789</v>
       </c>
       <c r="G3" t="n">
-        <v>32.732218172131</v>
+        <v>36.13317886880174</v>
       </c>
       <c r="H3" t="n">
         <v>3</v>
@@ -572,16 +572,16 @@
         <v>229.4375019646583</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9124940579766738</v>
+        <v>0.8266074428412484</v>
       </c>
       <c r="K3" t="n">
-        <v>0.8805834201955638</v>
+        <v>0.8336140462826277</v>
       </c>
       <c r="L3" t="n">
-        <v>0.7673652258821591</v>
+        <v>0.7977003278139295</v>
       </c>
       <c r="N3" t="n">
-        <v>0.4992128000000022</v>
+        <v>0.9678948999999974</v>
       </c>
       <c r="O3" t="n">
         <v>12.49761708641468</v>
@@ -608,7 +608,7 @@
         <v>35.32730948059873</v>
       </c>
       <c r="X3" t="n">
-        <v>0.193343899999995</v>
+        <v>0.2855381999999977</v>
       </c>
     </row>
     <row r="4">
@@ -649,7 +649,7 @@
         <v>0.7502997363077025</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2716589000000056</v>
+        <v>0.2777124000000057</v>
       </c>
     </row>
     <row r="5">
@@ -690,7 +690,7 @@
         <v>0.7371263675609472</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2504936999999998</v>
+        <v>0.2358201999999991</v>
       </c>
     </row>
     <row r="6">
@@ -734,7 +734,7 @@
         <v>14.9363833160678</v>
       </c>
       <c r="X6" t="n">
-        <v>0.2878898999999961</v>
+        <v>0.2658045000000016</v>
       </c>
     </row>
     <row r="7">
@@ -775,7 +775,7 @@
         <v>0.7294000163856171</v>
       </c>
       <c r="N7" t="n">
-        <v>0.5449338000000026</v>
+        <v>0.4692452000000031</v>
       </c>
       <c r="O7" t="n">
         <v>14.10479914623658</v>
@@ -802,7 +802,7 @@
         <v>55.81376649103811</v>
       </c>
       <c r="X7" t="n">
-        <v>0.4270886000000047</v>
+        <v>0.3977891999999983</v>
       </c>
     </row>
     <row r="8">
@@ -846,7 +846,7 @@
         <v>21.30428090617795</v>
       </c>
       <c r="X8" t="n">
-        <v>0.2266720000000007</v>
+        <v>0.2078437999999991</v>
       </c>
     </row>
     <row r="9">
@@ -921,7 +921,7 @@
         <v>0.6518587763807507</v>
       </c>
       <c r="N11" t="n">
-        <v>0.2583630999999968</v>
+        <v>0.2382264000000021</v>
       </c>
       <c r="O11" t="n">
         <v>8.201533682899196</v>
@@ -948,7 +948,7 @@
         <v>39.23836609572476</v>
       </c>
       <c r="X11" t="n">
-        <v>0.2176544000000007</v>
+        <v>0.2080446000000009</v>
       </c>
     </row>
     <row r="12">
@@ -992,7 +992,7 @@
         <v>22.93589661346448</v>
       </c>
       <c r="X12" t="n">
-        <v>0.2033862999999982</v>
+        <v>0.1614588999999995</v>
       </c>
     </row>
     <row r="13">
@@ -1036,7 +1036,7 @@
         <v>28.22636892663138</v>
       </c>
       <c r="X13" t="n">
-        <v>0.2045219000000031</v>
+        <v>0.1688521999999963</v>
       </c>
     </row>
     <row r="14">
@@ -1080,7 +1080,7 @@
         <v>45.51440616972206</v>
       </c>
       <c r="X14" t="n">
-        <v>0.1755707000000015</v>
+        <v>0.1557642999999942</v>
       </c>
     </row>
     <row r="15">
@@ -1121,7 +1121,7 @@
         <v>0.6343865750227973</v>
       </c>
       <c r="N15" t="n">
-        <v>0.4033848000000049</v>
+        <v>0.2979601999999986</v>
       </c>
       <c r="O15" t="n">
         <v>6.582434431888892</v>
@@ -1148,7 +1148,7 @@
         <v>33.0877576669921</v>
       </c>
       <c r="X15" t="n">
-        <v>0.8523867999999979</v>
+        <v>0.6715149999999994</v>
       </c>
     </row>
     <row r="16">
@@ -1189,7 +1189,7 @@
         <v>0.7412171406140956</v>
       </c>
       <c r="N16" t="n">
-        <v>0.2324069999999949</v>
+        <v>0.2542722999999967</v>
       </c>
       <c r="O16" t="n">
         <v>7.655540733280799</v>
@@ -1216,7 +1216,7 @@
         <v>38.69169951505916</v>
       </c>
       <c r="X16" t="n">
-        <v>0.3683844999999977</v>
+        <v>0.2776579999999953</v>
       </c>
     </row>
     <row r="17">
@@ -1257,7 +1257,7 @@
         <v>0.6174100361520386</v>
       </c>
       <c r="N17" t="n">
-        <v>0.1905969000000027</v>
+        <v>0.2043879000000004</v>
       </c>
       <c r="O17" t="n">
         <v>0.9719154228407159</v>
@@ -1278,7 +1278,7 @@
         <v>8.84430671396882</v>
       </c>
       <c r="X17" t="n">
-        <v>0.9703568999999987</v>
+        <v>4.407088799999997</v>
       </c>
     </row>
     <row r="18">
@@ -1336,7 +1336,7 @@
         <v>0.7218558184006625</v>
       </c>
       <c r="N19" t="n">
-        <v>0.2332853999999998</v>
+        <v>0.6540849000000009</v>
       </c>
       <c r="O19" t="n">
         <v>6.807915252906037</v>
@@ -1363,7 +1363,7 @@
         <v>46.80842965199952</v>
       </c>
       <c r="X19" t="n">
-        <v>0.4081564000000029</v>
+        <v>1.072646799999994</v>
       </c>
     </row>
     <row r="20">
@@ -1404,7 +1404,7 @@
         <v>0.5445504221440435</v>
       </c>
       <c r="N20" t="n">
-        <v>0.3659639999999982</v>
+        <v>1.070333599999998</v>
       </c>
       <c r="O20" t="n">
         <v>8.896998358735726</v>
@@ -1431,7 +1431,7 @@
         <v>55.20376541448184</v>
       </c>
       <c r="X20" t="n">
-        <v>0.1779270000000039</v>
+        <v>0.2058281999999991</v>
       </c>
     </row>
     <row r="21">
@@ -1472,7 +1472,7 @@
         <v>0.6954927850998559</v>
       </c>
       <c r="N21" t="n">
-        <v>0.2104149999999976</v>
+        <v>0.2663415999999899</v>
       </c>
       <c r="O21" t="n">
         <v>3.751261323481207</v>
@@ -1499,7 +1499,7 @@
         <v>39.34970828088581</v>
       </c>
       <c r="X21" t="n">
-        <v>0.2939124999999976</v>
+        <v>0.3587895000000003</v>
       </c>
     </row>
     <row r="22">
@@ -1540,7 +1540,7 @@
         <v>0.7145603697052624</v>
       </c>
       <c r="N22" t="n">
-        <v>0.3085018000000019</v>
+        <v>0.3609051000000107</v>
       </c>
       <c r="O22" t="n">
         <v>9.140000458889755</v>
@@ -1567,7 +1567,7 @@
         <v>57.53614698372837</v>
       </c>
       <c r="X22" t="n">
-        <v>0.1623935999999944</v>
+        <v>0.1707909999999941</v>
       </c>
     </row>
     <row r="23">
@@ -1608,7 +1608,7 @@
         <v>0.7885762479942238</v>
       </c>
       <c r="N23" t="n">
-        <v>0.1887624000000017</v>
+        <v>0.2335425999999927</v>
       </c>
       <c r="O23" t="n">
         <v>2.416074115714946</v>
@@ -1635,7 +1635,7 @@
         <v>35.13999931153762</v>
       </c>
       <c r="X23" t="n">
-        <v>0.1469149999999999</v>
+        <v>0.1578506000000033</v>
       </c>
     </row>
     <row r="24">
@@ -1676,7 +1676,7 @@
         <v>0.7673795573162669</v>
       </c>
       <c r="N24" t="n">
-        <v>0.3398419999999973</v>
+        <v>0.332782899999998</v>
       </c>
       <c r="O24" t="n">
         <v>14.07512366789098</v>
@@ -1703,7 +1703,7 @@
         <v>46.39416756456535</v>
       </c>
       <c r="X24" t="n">
-        <v>0.1983905999999962</v>
+        <v>0.1971659000000017</v>
       </c>
     </row>
     <row r="25">
@@ -1744,7 +1744,7 @@
         <v>0.5893135288182765</v>
       </c>
       <c r="N25" t="n">
-        <v>0.2194961999999947</v>
+        <v>0.2389526999999987</v>
       </c>
     </row>
     <row r="26">
@@ -1785,7 +1785,7 @@
         <v>0.6289246745312014</v>
       </c>
       <c r="N26" t="n">
-        <v>0.3090657999999991</v>
+        <v>0.2935942999999952</v>
       </c>
       <c r="O26" t="n">
         <v>11.84910243788312</v>
@@ -1812,7 +1812,7 @@
         <v>50.2525579907014</v>
       </c>
       <c r="X26" t="n">
-        <v>0.2517217999999986</v>
+        <v>0.2763700999999941</v>
       </c>
     </row>
     <row r="27">
@@ -1870,7 +1870,7 @@
         <v>0.5999804683154401</v>
       </c>
       <c r="N28" t="n">
-        <v>0.3078181000000058</v>
+        <v>0.3313120000000112</v>
       </c>
       <c r="O28" t="n">
         <v>2.786952465828485</v>
@@ -1894,7 +1894,7 @@
         <v>56.59696015007074</v>
       </c>
       <c r="X28" t="n">
-        <v>0.2405296999999962</v>
+        <v>0.2615523999999994</v>
       </c>
     </row>
     <row r="29">
@@ -1935,7 +1935,7 @@
         <v>0.71888906807707</v>
       </c>
       <c r="N29" t="n">
-        <v>0.3542256000000066</v>
+        <v>0.3919108999999992</v>
       </c>
       <c r="O29" t="n">
         <v>5.904264218426784</v>
@@ -1962,7 +1962,7 @@
         <v>51.96646310751828</v>
       </c>
       <c r="X29" t="n">
-        <v>0.8636651000000057</v>
+        <v>0.6536406999999969</v>
       </c>
     </row>
     <row r="30">
@@ -2003,7 +2003,7 @@
         <v>0.5786847596367948</v>
       </c>
       <c r="N30" t="n">
-        <v>0.2890650000000079</v>
+        <v>0.3546708000000081</v>
       </c>
       <c r="O30" t="n">
         <v>13.55025677870883</v>
@@ -2030,7 +2030,7 @@
         <v>58.1407327462955</v>
       </c>
       <c r="X30" t="n">
-        <v>0.2889883999999938</v>
+        <v>0.2300856000000095</v>
       </c>
     </row>
     <row r="31">
@@ -2071,7 +2071,7 @@
         <v>0.6800036212002831</v>
       </c>
       <c r="N31" t="n">
-        <v>0.3039978000000048</v>
+        <v>0.3058254000000034</v>
       </c>
       <c r="O31" t="n">
         <v>9.885791273851719</v>
@@ -2098,7 +2098,7 @@
         <v>36.56763280519203</v>
       </c>
       <c r="X31" t="n">
-        <v>0.2087596000000076</v>
+        <v>0.1953960999999964</v>
       </c>
     </row>
     <row r="32">
@@ -2139,7 +2139,7 @@
         <v>0.8022139622054861</v>
       </c>
       <c r="N32" t="n">
-        <v>0.423135000000002</v>
+        <v>0.3588330999999982</v>
       </c>
       <c r="O32" t="n">
         <v>11.50243435678393</v>
@@ -2166,7 +2166,7 @@
         <v>59.48210624045475</v>
       </c>
       <c r="X32" t="n">
-        <v>0.2608871999999991</v>
+        <v>0.2557520000000011</v>
       </c>
     </row>
     <row r="33">
@@ -2227,7 +2227,7 @@
         <v>50.86138544009225</v>
       </c>
       <c r="X34" t="n">
-        <v>0.4242200999999994</v>
+        <v>0.3769130000000018</v>
       </c>
     </row>
     <row r="35">
@@ -2271,7 +2271,7 @@
         <v>23.18246951406661</v>
       </c>
       <c r="X35" t="n">
-        <v>0.1588536000000005</v>
+        <v>0.1645892000000089</v>
       </c>
     </row>
     <row r="36">
@@ -2315,7 +2315,7 @@
         <v>16.43928921731816</v>
       </c>
       <c r="X36" t="n">
-        <v>0.2041973999999982</v>
+        <v>0.2077625999999952</v>
       </c>
     </row>
     <row r="37">
@@ -2356,7 +2356,7 @@
         <v>0.586159877402691</v>
       </c>
       <c r="N37" t="n">
-        <v>0.3063585000000018</v>
+        <v>0.3348988000000048</v>
       </c>
       <c r="O37" t="n">
         <v>6.954434984205963</v>
@@ -2383,7 +2383,7 @@
         <v>49.846764840275</v>
       </c>
       <c r="X37" t="n">
-        <v>0.1518092999999965</v>
+        <v>0.1536124999999942</v>
       </c>
     </row>
     <row r="38">
@@ -2441,7 +2441,7 @@
         <v>55.54071084240474</v>
       </c>
       <c r="X39" t="n">
-        <v>0.5833504000000005</v>
+        <v>0.6438468000000057</v>
       </c>
     </row>
     <row r="40">
@@ -2482,7 +2482,7 @@
         <v>0.5614734246846576</v>
       </c>
       <c r="N40" t="n">
-        <v>0.6307156999999961</v>
+        <v>0.6520766000000009</v>
       </c>
     </row>
     <row r="41">
@@ -2523,7 +2523,7 @@
         <v>0.952559957246823</v>
       </c>
       <c r="N41" t="n">
-        <v>0.2490895999999907</v>
+        <v>0.2717001999999979</v>
       </c>
       <c r="O41" t="n">
         <v>5.77109258684423</v>
@@ -2550,7 +2550,7 @@
         <v>55.33722413506393</v>
       </c>
       <c r="X41" t="n">
-        <v>0.1361961000000065</v>
+        <v>0.1773760000000095</v>
       </c>
     </row>
     <row r="42">
@@ -2591,7 +2591,7 @@
         <v>0.7050371273664621</v>
       </c>
       <c r="N42" t="n">
-        <v>0.2546674000000024</v>
+        <v>0.2845427000000029</v>
       </c>
       <c r="O42" t="n">
         <v>1.075604586092394</v>
@@ -2612,7 +2612,7 @@
         <v>19.74265575570439</v>
       </c>
       <c r="X42" t="n">
-        <v>0.4596289999999925</v>
+        <v>0.4897109000000057</v>
       </c>
     </row>
     <row r="43">
@@ -2670,7 +2670,7 @@
         <v>0.8800581615536265</v>
       </c>
       <c r="N44" t="n">
-        <v>0.2592863000000136</v>
+        <v>0.2968840999999998</v>
       </c>
       <c r="O44" t="n">
         <v>9.84163207654866</v>
@@ -2697,7 +2697,7 @@
         <v>40.66306484336559</v>
       </c>
       <c r="X44" t="n">
-        <v>0.5271022999999957</v>
+        <v>0.5466957999999948</v>
       </c>
     </row>
     <row r="45">
@@ -2741,7 +2741,7 @@
         <v>56.30770522182081</v>
       </c>
       <c r="X45" t="n">
-        <v>0.1700440999999984</v>
+        <v>0.180628200000001</v>
       </c>
     </row>
     <row r="46">
@@ -2785,7 +2785,7 @@
         <v>59.04088714732057</v>
       </c>
       <c r="X46" t="n">
-        <v>0.2904535999999922</v>
+        <v>0.3211270999999982</v>
       </c>
     </row>
     <row r="47">
@@ -2843,7 +2843,7 @@
         <v>0.7881604774505526</v>
       </c>
       <c r="N48" t="n">
-        <v>0.2820542000000046</v>
+        <v>0.322967300000002</v>
       </c>
       <c r="O48" t="n">
         <v>11.62392031857079</v>
@@ -2870,7 +2870,7 @@
         <v>46.45972825576388</v>
       </c>
       <c r="X48" t="n">
-        <v>0.2307234000000022</v>
+        <v>0.2440399999999983</v>
       </c>
     </row>
     <row r="49">
@@ -2914,7 +2914,7 @@
         <v>59.55296311242046</v>
       </c>
       <c r="X49" t="n">
-        <v>0.3866277999999994</v>
+        <v>0.4046818000000059</v>
       </c>
     </row>
     <row r="50">
@@ -2989,7 +2989,7 @@
         <v>0.7134380378238956</v>
       </c>
       <c r="N52" t="n">
-        <v>0.3077657000000045</v>
+        <v>0.3239482999999979</v>
       </c>
       <c r="O52" t="n">
         <v>13.47114947668005</v>
@@ -3016,7 +3016,7 @@
         <v>47.30506405382903</v>
       </c>
       <c r="X52" t="n">
-        <v>0.3021984999999887</v>
+        <v>0.2989891</v>
       </c>
     </row>
     <row r="53">
@@ -3057,7 +3057,7 @@
         <v>0.7574887991113182</v>
       </c>
       <c r="N53" t="n">
-        <v>0.8670225999999985</v>
+        <v>1.025766300000001</v>
       </c>
       <c r="O53" t="n">
         <v>11.31119466449514</v>
@@ -3084,7 +3084,7 @@
         <v>48.57156942197514</v>
       </c>
       <c r="X53" t="n">
-        <v>0.3409987000000001</v>
+        <v>0.2828942999999953</v>
       </c>
     </row>
     <row r="54">
@@ -3125,7 +3125,7 @@
         <v>0.7454613074654333</v>
       </c>
       <c r="N54" t="n">
-        <v>0.2396370000000019</v>
+        <v>0.2712860999999975</v>
       </c>
       <c r="O54" t="n">
         <v>11.65213715318634</v>
@@ -3152,7 +3152,7 @@
         <v>38.71382560609396</v>
       </c>
       <c r="X54" t="n">
-        <v>0.2324710999999979</v>
+        <v>0.2477413000000013</v>
       </c>
     </row>
     <row r="55">
@@ -3261,7 +3261,7 @@
         <v>0.5572668092236944</v>
       </c>
       <c r="N59" t="n">
-        <v>0.3453062999999901</v>
+        <v>0.3162820999999951</v>
       </c>
       <c r="O59" t="n">
         <v>13.10461298038586</v>
@@ -3288,7 +3288,7 @@
         <v>42.88304695540518</v>
       </c>
       <c r="X59" t="n">
-        <v>0.2468679999999921</v>
+        <v>0.2544809000000043</v>
       </c>
     </row>
     <row r="60">
@@ -3329,7 +3329,7 @@
         <v>0.6309847701756546</v>
       </c>
       <c r="N60" t="n">
-        <v>0.2906928999999963</v>
+        <v>0.3416500000000013</v>
       </c>
     </row>
     <row r="61">
@@ -3370,7 +3370,7 @@
         <v>0.7867007228834226</v>
       </c>
       <c r="N61" t="n">
-        <v>0.303648999999993</v>
+        <v>0.3317207000000053</v>
       </c>
       <c r="O61" t="n">
         <v>9.987862134498778</v>
@@ -3397,7 +3397,7 @@
         <v>53.77820152627504</v>
       </c>
       <c r="X61" t="n">
-        <v>0.2308053999999942</v>
+        <v>0.2542547999999982</v>
       </c>
     </row>
     <row r="62">
@@ -3441,7 +3441,7 @@
         <v>45.23882636811368</v>
       </c>
       <c r="X62" t="n">
-        <v>0.1711808000000019</v>
+        <v>0.1837413000000083</v>
       </c>
     </row>
     <row r="63">
@@ -3502,7 +3502,7 @@
         <v>37.56753887726268</v>
       </c>
       <c r="X64" t="n">
-        <v>0.2929305999999912</v>
+        <v>0.2833382999999969</v>
       </c>
     </row>
     <row r="65">
@@ -3521,6 +3521,30 @@
       <c r="E65" t="n">
         <v>2114</v>
       </c>
+      <c r="F65" t="n">
+        <v>10.50526734053436</v>
+      </c>
+      <c r="G65" t="n">
+        <v>32.65886219855242</v>
+      </c>
+      <c r="H65" t="n">
+        <v>3</v>
+      </c>
+      <c r="I65" t="n">
+        <v>165.2283969657749</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.6045626252366123</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.6582476994966975</v>
+      </c>
+      <c r="L65" t="n">
+        <v>0.7664820620288616</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0.6651762000000048</v>
+      </c>
       <c r="O65" t="n">
         <v>3.509165855753642</v>
       </c>
@@ -3540,7 +3564,7 @@
         <v>48.09420178143387</v>
       </c>
       <c r="X65" t="n">
-        <v>0.6782733999999948</v>
+        <v>0.6834201000000064</v>
       </c>
     </row>
     <row r="66">
@@ -3581,7 +3605,7 @@
         <v>0.9568050625003772</v>
       </c>
       <c r="N66" t="n">
-        <v>0.7905114999999938</v>
+        <v>0.3265185999999858</v>
       </c>
       <c r="O66" t="n">
         <v>8.339759165045479</v>
@@ -3608,7 +3632,7 @@
         <v>35.08335700389608</v>
       </c>
       <c r="X66" t="n">
-        <v>1.107742799999997</v>
+        <v>0.3544724000000201</v>
       </c>
     </row>
     <row r="67">
@@ -3652,7 +3676,7 @@
         <v>57.97587948174441</v>
       </c>
       <c r="X67" t="n">
-        <v>0.2037416000000007</v>
+        <v>0.235990600000008</v>
       </c>
     </row>
     <row r="68">
@@ -3693,7 +3717,7 @@
         <v>0.7520959774273354</v>
       </c>
       <c r="N68" t="n">
-        <v>0.4320928000000066</v>
+        <v>0.476895600000006</v>
       </c>
       <c r="O68" t="n">
         <v>12.42246620264435</v>
@@ -3720,7 +3744,7 @@
         <v>29.166953977866</v>
       </c>
       <c r="X68" t="n">
-        <v>0.2801455999999973</v>
+        <v>0.3223867000000098</v>
       </c>
     </row>
     <row r="69">
@@ -3761,7 +3785,7 @@
         <v>0.6859577668551914</v>
       </c>
       <c r="N69" t="n">
-        <v>0.3248198000000002</v>
+        <v>0.3228857000000005</v>
       </c>
     </row>
     <row r="70">
@@ -3819,7 +3843,7 @@
         <v>0.7502103559470656</v>
       </c>
       <c r="N71" t="n">
-        <v>0.2855457000000001</v>
+        <v>0.28957410000001</v>
       </c>
       <c r="O71" t="n">
         <v>7.572412157140905</v>
@@ -3846,7 +3870,7 @@
         <v>29.13443686836865</v>
       </c>
       <c r="X71" t="n">
-        <v>0.1836291000000045</v>
+        <v>0.1800479000000053</v>
       </c>
     </row>
     <row r="72">
@@ -3904,7 +3928,7 @@
         <v>0.7489480931143536</v>
       </c>
       <c r="N73" t="n">
-        <v>0.299043999999995</v>
+        <v>0.2952327000000139</v>
       </c>
       <c r="O73" t="n">
         <v>15.80939597182488</v>
@@ -3931,7 +3955,7 @@
         <v>53.65016599065109</v>
       </c>
       <c r="X73" t="n">
-        <v>0.4593311</v>
+        <v>0.3378423999999995</v>
       </c>
     </row>
     <row r="74">
@@ -3969,7 +3993,7 @@
         <v>28.6141737287187</v>
       </c>
       <c r="X74" t="n">
-        <v>1.09838400000001</v>
+        <v>0.7718134999999791</v>
       </c>
     </row>
     <row r="75">
@@ -4010,7 +4034,7 @@
         <v>47.40962670901428</v>
       </c>
       <c r="X75" t="n">
-        <v>0.4944398999999891</v>
+        <v>0.3962062999999887</v>
       </c>
     </row>
     <row r="76">
@@ -4051,7 +4075,7 @@
         <v>0.6945818775739012</v>
       </c>
       <c r="N76" t="n">
-        <v>0.3176570000000112</v>
+        <v>0.3049416000000065</v>
       </c>
       <c r="O76" t="n">
         <v>12.09781490595968</v>
@@ -4078,7 +4102,7 @@
         <v>56.38251254024499</v>
       </c>
       <c r="X76" t="n">
-        <v>0.1836643000000038</v>
+        <v>0.1725917999999922</v>
       </c>
     </row>
     <row r="77">
@@ -4119,7 +4143,7 @@
         <v>0.765234274966803</v>
       </c>
       <c r="N77" t="n">
-        <v>0.3123882000000151</v>
+        <v>0.3148227000000077</v>
       </c>
       <c r="O77" t="n">
         <v>10.57013802622273</v>
@@ -4146,7 +4170,7 @@
         <v>53.89571795561051</v>
       </c>
       <c r="X77" t="n">
-        <v>0.209526000000011</v>
+        <v>0.1999768999999958</v>
       </c>
     </row>
     <row r="78">
@@ -4187,7 +4211,7 @@
         <v>0.6847391850735041</v>
       </c>
       <c r="N78" t="n">
-        <v>0.4066971999999964</v>
+        <v>0.296871799999991</v>
       </c>
       <c r="O78" t="n">
         <v>11.06833403200247</v>
@@ -4214,7 +4238,7 @@
         <v>40.24225044544824</v>
       </c>
       <c r="X78" t="n">
-        <v>0.1887605000000008</v>
+        <v>0.2292611999999963</v>
       </c>
     </row>
     <row r="79">
@@ -4255,7 +4279,7 @@
         <v>0.7301596146116747</v>
       </c>
       <c r="N79" t="n">
-        <v>0.4491710000000069</v>
+        <v>0.4525038000000166</v>
       </c>
     </row>
     <row r="80">
@@ -4330,7 +4354,7 @@
         <v>0.7327754278658019</v>
       </c>
       <c r="N82" t="n">
-        <v>0.2529896000000065</v>
+        <v>0.2622953000000052</v>
       </c>
       <c r="O82" t="n">
         <v>10.61089507863382</v>
@@ -4357,7 +4381,7 @@
         <v>57.9426278929609</v>
       </c>
       <c r="X82" t="n">
-        <v>0.3204867999999976</v>
+        <v>0.3019091000000174</v>
       </c>
     </row>
     <row r="83">
@@ -4398,7 +4422,7 @@
         <v>0.7764527465325202</v>
       </c>
       <c r="N83" t="n">
-        <v>0.3613784000000066</v>
+        <v>0.3282921999999928</v>
       </c>
       <c r="O83" t="n">
         <v>13.04264621425495</v>
@@ -4425,7 +4449,7 @@
         <v>54.41365671433891</v>
       </c>
       <c r="X83" t="n">
-        <v>0.3112013999999874</v>
+        <v>0.2983462999999915</v>
       </c>
     </row>
     <row r="84">
@@ -4466,7 +4490,7 @@
         <v>0.7137209245069888</v>
       </c>
       <c r="N84" t="n">
-        <v>0.3214187000000095</v>
+        <v>0.3621665999999948</v>
       </c>
       <c r="O84" t="n">
         <v>14.26093881179648</v>
@@ -4493,7 +4517,7 @@
         <v>53.64682303198879</v>
       </c>
       <c r="X84" t="n">
-        <v>0.2208834999999851</v>
+        <v>0.2421436999999855</v>
       </c>
     </row>
     <row r="85">
@@ -4537,7 +4561,7 @@
         <v>44.07957798744502</v>
       </c>
       <c r="X85" t="n">
-        <v>0.2096298999999817</v>
+        <v>0.2073916999999881</v>
       </c>
     </row>
     <row r="86">
@@ -4595,7 +4619,7 @@
         <v>0.5196037362405583</v>
       </c>
       <c r="N87" t="n">
-        <v>0.2612530000000106</v>
+        <v>0.2765635000000088</v>
       </c>
       <c r="O87" t="n">
         <v>10.39177272279499</v>
@@ -4622,7 +4646,7 @@
         <v>54.746075089854</v>
       </c>
       <c r="X87" t="n">
-        <v>0.7432602000000088</v>
+        <v>0.7424371000000178</v>
       </c>
     </row>
     <row r="88">
@@ -4663,7 +4687,7 @@
         <v>0.6765364810570895</v>
       </c>
       <c r="N88" t="n">
-        <v>0.2313745000000154</v>
+        <v>0.2751312999999982</v>
       </c>
     </row>
     <row r="89">
@@ -4724,7 +4748,7 @@
         <v>24.87998961051136</v>
       </c>
       <c r="X90" t="n">
-        <v>0.1650218000000052</v>
+        <v>0.1672095999999783</v>
       </c>
     </row>
     <row r="91">
@@ -4816,7 +4840,7 @@
         <v>0.7258996951481946</v>
       </c>
       <c r="N94" t="n">
-        <v>0.2591302999999812</v>
+        <v>0.2820537000000058</v>
       </c>
       <c r="O94" t="n">
         <v>14.34155742807301</v>
@@ -4843,7 +4867,7 @@
         <v>51.00140785089667</v>
       </c>
       <c r="X94" t="n">
-        <v>0.2326786000000141</v>
+        <v>0.2334770000000219</v>
       </c>
     </row>
     <row r="95">
@@ -4921,7 +4945,7 @@
         <v>48.63095956622971</v>
       </c>
       <c r="X97" t="n">
-        <v>0.2743995000000155</v>
+        <v>0.276834899999983</v>
       </c>
     </row>
     <row r="98">
@@ -4962,7 +4986,7 @@
         <v>0.6110729467681992</v>
       </c>
       <c r="N98" t="n">
-        <v>0.3396310999999912</v>
+        <v>0.3595049000000188</v>
       </c>
       <c r="O98" t="n">
         <v>9.03843260641283</v>
@@ -4989,7 +5013,7 @@
         <v>55.84863048047959</v>
       </c>
       <c r="X98" t="n">
-        <v>0.5978680999999995</v>
+        <v>0.6132888000000207</v>
       </c>
     </row>
     <row r="99">
@@ -5030,7 +5054,7 @@
         <v>0.6401584182965168</v>
       </c>
       <c r="N99" t="n">
-        <v>0.2905568000000187</v>
+        <v>0.3065887000000203</v>
       </c>
       <c r="O99" t="n">
         <v>5.851133559999255</v>
@@ -5057,7 +5081,7 @@
         <v>42.33478532309601</v>
       </c>
       <c r="X99" t="n">
-        <v>0.2516655999999955</v>
+        <v>0.2173242000000073</v>
       </c>
     </row>
     <row r="100">
@@ -5118,7 +5142,7 @@
         <v>52.66508630199286</v>
       </c>
       <c r="X101" t="n">
-        <v>0.1693952999999908</v>
+        <v>0.1702390000000094</v>
       </c>
     </row>
     <row r="102">
@@ -5159,7 +5183,7 @@
         <v>0.5490618954190731</v>
       </c>
       <c r="N102" t="n">
-        <v>0.3196444000000156</v>
+        <v>0.3311808999999926</v>
       </c>
       <c r="O102" t="n">
         <v>10.4053991511358</v>
@@ -5186,7 +5210,7 @@
         <v>44.84836519228753</v>
       </c>
       <c r="X102" t="n">
-        <v>0.7030838999999958</v>
+        <v>0.7215951999999959</v>
       </c>
     </row>
     <row r="103">
@@ -5227,7 +5251,7 @@
         <v>0.7592616329955325</v>
       </c>
       <c r="N103" t="n">
-        <v>0.2144890000000146</v>
+        <v>0.2295500999999831</v>
       </c>
       <c r="O103" t="n">
         <v>4.792432876864117</v>
@@ -5254,7 +5278,7 @@
         <v>39.9419958169031</v>
       </c>
       <c r="X103" t="n">
-        <v>0.1610058999999922</v>
+        <v>0.1618191000000024</v>
       </c>
     </row>
     <row r="104">
@@ -5298,7 +5322,7 @@
         <v>23.11590132617221</v>
       </c>
       <c r="X104" t="n">
-        <v>0.2203796000000011</v>
+        <v>0.2182783000000086</v>
       </c>
     </row>
     <row r="105">
@@ -5356,7 +5380,7 @@
         <v>0.5630212263897855</v>
       </c>
       <c r="N106" t="n">
-        <v>0.2832903999999985</v>
+        <v>0.3070486000000017</v>
       </c>
       <c r="O106" t="n">
         <v>9.093567248490176</v>
@@ -5383,7 +5407,7 @@
         <v>52.2049780764026</v>
       </c>
       <c r="X106" t="n">
-        <v>0.2371751000000017</v>
+        <v>0.2808051000000091</v>
       </c>
     </row>
     <row r="107">
@@ -5427,7 +5451,7 @@
         <v>58.87600731870526</v>
       </c>
       <c r="X107" t="n">
-        <v>0.3948299999999847</v>
+        <v>0.4058542000000216</v>
       </c>
     </row>
     <row r="108">
@@ -5468,7 +5492,7 @@
         <v>58.65767156528716</v>
       </c>
       <c r="X108" t="n">
-        <v>0.5570453999999927</v>
+        <v>0.5657315999999923</v>
       </c>
     </row>
     <row r="109">
@@ -5506,7 +5530,7 @@
         <v>11.82465668211256</v>
       </c>
       <c r="X109" t="n">
-        <v>0.2919445999999937</v>
+        <v>0.3007551999999976</v>
       </c>
     </row>
     <row r="110">
@@ -5564,7 +5588,7 @@
         <v>0.7693640756993421</v>
       </c>
       <c r="N111" t="n">
-        <v>0.2696454000000017</v>
+        <v>0.2804232000000013</v>
       </c>
       <c r="O111" t="n">
         <v>6.18550542330814</v>
@@ -5588,7 +5612,7 @@
         <v>17.82265020858767</v>
       </c>
       <c r="X111" t="n">
-        <v>0.2004991999999959</v>
+        <v>0.1878537000000051</v>
       </c>
     </row>
     <row r="112">
@@ -5629,7 +5653,7 @@
         <v>0.7072238685633592</v>
       </c>
       <c r="N112" t="n">
-        <v>0.353026199999988</v>
+        <v>0.3796472999999878</v>
       </c>
     </row>
     <row r="113">
@@ -5670,7 +5694,7 @@
         <v>0.563446518934809</v>
       </c>
       <c r="N113" t="n">
-        <v>0.2834584999999947</v>
+        <v>0.3065610000000163</v>
       </c>
     </row>
     <row r="114">
@@ -5711,7 +5735,7 @@
         <v>0.7176673529978116</v>
       </c>
       <c r="N114" t="n">
-        <v>0.2583320000000242</v>
+        <v>0.2864722999999856</v>
       </c>
       <c r="O114" t="n">
         <v>13.10792546632432</v>
@@ -5738,7 +5762,7 @@
         <v>54.58696210380293</v>
       </c>
       <c r="X114" t="n">
-        <v>0.2251486000000114</v>
+        <v>0.2315764999999885</v>
       </c>
     </row>
     <row r="115">
@@ -5779,7 +5803,7 @@
         <v>0.6293457841602239</v>
       </c>
       <c r="N115" t="n">
-        <v>0.2985704000000169</v>
+        <v>0.3426165000000196</v>
       </c>
       <c r="O115" t="n">
         <v>9.362845680181721</v>
@@ -5806,7 +5830,7 @@
         <v>53.19096702890215</v>
       </c>
       <c r="X115" t="n">
-        <v>0.3020305000000008</v>
+        <v>0.3105028999999888</v>
       </c>
     </row>
     <row r="116">
@@ -5847,7 +5871,7 @@
         <v>0.6512815729622599</v>
       </c>
       <c r="N116" t="n">
-        <v>0.6290228999999954</v>
+        <v>0.6432823000000099</v>
       </c>
       <c r="O116" t="n">
         <v>12.17253832135357</v>
@@ -5874,7 +5898,7 @@
         <v>41.10830087359403</v>
       </c>
       <c r="X116" t="n">
-        <v>1.150789299999985</v>
+        <v>1.087845299999998</v>
       </c>
     </row>
     <row r="117">
@@ -5935,7 +5959,7 @@
         <v>15.29120368022069</v>
       </c>
       <c r="X118" t="n">
-        <v>0.2738549000000035</v>
+        <v>0.2634992000000125</v>
       </c>
     </row>
     <row r="119">
@@ -6027,7 +6051,7 @@
         <v>0.7853935829475021</v>
       </c>
       <c r="N122" t="n">
-        <v>0.3353623000000141</v>
+        <v>0.3421936000000017</v>
       </c>
       <c r="O122" t="n">
         <v>16.54905738559482</v>
@@ -6054,7 +6078,7 @@
         <v>45.55108687726033</v>
       </c>
       <c r="X122" t="n">
-        <v>0.4158081999999865</v>
+        <v>0.3519211999999925</v>
       </c>
     </row>
     <row r="123">
@@ -6095,7 +6119,7 @@
         <v>0.5550880981211724</v>
       </c>
       <c r="N123" t="n">
-        <v>0.4364977999999837</v>
+        <v>0.4538570999999934</v>
       </c>
       <c r="O123" t="n">
         <v>11.10295649589333</v>
@@ -6122,7 +6146,7 @@
         <v>59.55105576581059</v>
       </c>
       <c r="X123" t="n">
-        <v>0.319972899999982</v>
+        <v>0.3212790000000041</v>
       </c>
     </row>
     <row r="124">
@@ -6183,7 +6207,7 @@
         <v>45.09149429746742</v>
       </c>
       <c r="X125" t="n">
-        <v>0.1472372000000064</v>
+        <v>0.1445456000000149</v>
       </c>
     </row>
     <row r="126">
@@ -6227,7 +6251,7 @@
         <v>53.87732308547976</v>
       </c>
       <c r="X126" t="n">
-        <v>0.3331639000000166</v>
+        <v>0.3458170999999766</v>
       </c>
     </row>
     <row r="127">
@@ -6285,7 +6309,7 @@
         <v>0.7659442343454008</v>
       </c>
       <c r="N128" t="n">
-        <v>0.3970567000000074</v>
+        <v>0.4203693999999984</v>
       </c>
     </row>
     <row r="129">
@@ -6329,7 +6353,7 @@
         <v>53.43539695172467</v>
       </c>
       <c r="X129" t="n">
-        <v>0.2289054999999962</v>
+        <v>0.2326856000000248</v>
       </c>
     </row>
     <row r="130">
@@ -6370,7 +6394,7 @@
         <v>0.7759910627655574</v>
       </c>
       <c r="N130" t="n">
-        <v>0.2743179999999938</v>
+        <v>0.2836877000000015</v>
       </c>
       <c r="O130" t="n">
         <v>8.105205003386365</v>
@@ -6397,7 +6421,7 @@
         <v>40.19682577529397</v>
       </c>
       <c r="X130" t="n">
-        <v>0.4039003000000037</v>
+        <v>0.3777197999999942</v>
       </c>
     </row>
     <row r="131">
@@ -6438,7 +6462,7 @@
         <v>0.569229075708252</v>
       </c>
       <c r="N131" t="n">
-        <v>0.4187319999999772</v>
+        <v>0.4330954000000133</v>
       </c>
     </row>
     <row r="132">
@@ -6516,7 +6540,7 @@
         <v>31.47988333200948</v>
       </c>
       <c r="X134" t="n">
-        <v>0.1466350999999975</v>
+        <v>0.1413768999999832</v>
       </c>
     </row>
     <row r="135">
@@ -6557,7 +6581,7 @@
         <v>0.66177104046478</v>
       </c>
       <c r="N135" t="n">
-        <v>0.2657497000000149</v>
+        <v>0.2844071000000099</v>
       </c>
       <c r="O135" t="n">
         <v>3.510807356990619</v>
@@ -6581,7 +6605,7 @@
         <v>58.56807053357409</v>
       </c>
       <c r="X135" t="n">
-        <v>0.9814882000000011</v>
+        <v>1.056798500000014</v>
       </c>
     </row>
     <row r="136">
@@ -6622,7 +6646,7 @@
         <v>0.5582792116201171</v>
       </c>
       <c r="N136" t="n">
-        <v>0.2991735000000233</v>
+        <v>0.3524252999999931</v>
       </c>
       <c r="O136" t="n">
         <v>11.51789739635981</v>
@@ -6649,7 +6673,7 @@
         <v>45.39224590383571</v>
       </c>
       <c r="X136" t="n">
-        <v>0.1578278000000068</v>
+        <v>0.1589243999999894</v>
       </c>
     </row>
     <row r="137">
@@ -6724,7 +6748,7 @@
         <v>0.6139147613972666</v>
       </c>
       <c r="N139" t="n">
-        <v>0.2398923999999738</v>
+        <v>0.2550736000000029</v>
       </c>
       <c r="O139" t="n">
         <v>8.432087112100337</v>
@@ -6751,7 +6775,7 @@
         <v>41.42690979209499</v>
       </c>
       <c r="X139" t="n">
-        <v>0.1620436999999981</v>
+        <v>0.1741823000000124</v>
       </c>
     </row>
     <row r="140">
@@ -6789,7 +6813,7 @@
         <v>55.42043637027763</v>
       </c>
       <c r="X140" t="n">
-        <v>0.4915005000000008</v>
+        <v>0.4561355000000162</v>
       </c>
     </row>
     <row r="141">
@@ -6830,7 +6854,7 @@
         <v>0.6729219362534257</v>
       </c>
       <c r="N141" t="n">
-        <v>0.2888025000000027</v>
+        <v>0.3013986999999929</v>
       </c>
       <c r="O141" t="n">
         <v>11.87508252603232</v>
@@ -6857,7 +6881,7 @@
         <v>52.1155866369736</v>
       </c>
       <c r="X141" t="n">
-        <v>0.2911377000000073</v>
+        <v>0.3035380999999973</v>
       </c>
     </row>
     <row r="142">
@@ -6918,7 +6942,7 @@
         <v>54.36371412701669</v>
       </c>
       <c r="X143" t="n">
-        <v>0.1255095999999867</v>
+        <v>0.1231388999999865</v>
       </c>
     </row>
     <row r="144">
@@ -6976,7 +7000,7 @@
         <v>0.8558606885423212</v>
       </c>
       <c r="N145" t="n">
-        <v>0.2936356999999816</v>
+        <v>0.3145199000000218</v>
       </c>
     </row>
     <row r="146">
@@ -7068,7 +7092,7 @@
         <v>0.7960451662319317</v>
       </c>
       <c r="N149" t="n">
-        <v>0.3059594000000061</v>
+        <v>0.3124100999999939</v>
       </c>
       <c r="O149" t="n">
         <v>12.91273953453267</v>
@@ -7095,7 +7119,7 @@
         <v>53.81741578465426</v>
       </c>
       <c r="X149" t="n">
-        <v>0.1592491000000109</v>
+        <v>0.1948972999999796</v>
       </c>
     </row>
     <row r="150">
@@ -7136,7 +7160,7 @@
         <v>0.6054464091559779</v>
       </c>
       <c r="N150" t="n">
-        <v>0.3847477999999853</v>
+        <v>0.410746300000028</v>
       </c>
       <c r="O150" t="n">
         <v>6.277237197854125</v>
@@ -7163,7 +7187,7 @@
         <v>56.18642606325272</v>
       </c>
       <c r="X150" t="n">
-        <v>0.6561231999999961</v>
+        <v>0.6073516000000154</v>
       </c>
     </row>
     <row r="151">
@@ -7204,7 +7228,7 @@
         <v>0.6297107645357374</v>
       </c>
       <c r="N151" t="n">
-        <v>0.3630057999999963</v>
+        <v>0.4191595000000063</v>
       </c>
       <c r="O151" t="n">
         <v>10.52431731741115</v>
@@ -7231,7 +7255,7 @@
         <v>46.43913516348482</v>
       </c>
       <c r="X151" t="n">
-        <v>0.2792574000000059</v>
+        <v>0.199483999999984</v>
       </c>
     </row>
     <row r="152">
@@ -7289,7 +7313,7 @@
         <v>0.8416314569403841</v>
       </c>
       <c r="N153" t="n">
-        <v>0.2832270000000108</v>
+        <v>0.3016506000000163</v>
       </c>
       <c r="O153" t="n">
         <v>12.85689708840115</v>
@@ -7316,7 +7340,7 @@
         <v>59.79472728984803</v>
       </c>
       <c r="X153" t="n">
-        <v>0.2319780999999921</v>
+        <v>0.2269661999999926</v>
       </c>
     </row>
     <row r="154">
@@ -7357,7 +7381,7 @@
         <v>0.8351023701043093</v>
       </c>
       <c r="N154" t="n">
-        <v>0.4303371999999968</v>
+        <v>0.3451029999999946</v>
       </c>
       <c r="O154" t="n">
         <v>9.247466821858925</v>
@@ -7381,7 +7405,7 @@
         <v>19.96918238391919</v>
       </c>
       <c r="X154" t="n">
-        <v>0.1716726999999878</v>
+        <v>0.1680581000000245</v>
       </c>
     </row>
     <row r="155">
@@ -7459,7 +7483,7 @@
         <v>46.82679492343993</v>
       </c>
       <c r="X157" t="n">
-        <v>0.6129678000000069</v>
+        <v>0.600037599999979</v>
       </c>
     </row>
     <row r="158">
@@ -7500,7 +7524,7 @@
         <v>0.9284176031828719</v>
       </c>
       <c r="N158" t="n">
-        <v>0.2895212999999899</v>
+        <v>0.3093284000000267</v>
       </c>
       <c r="O158" t="n">
         <v>15.74351056565251</v>
@@ -7527,7 +7551,7 @@
         <v>54.79504122342809</v>
       </c>
       <c r="X158" t="n">
-        <v>0.2802376999999865</v>
+        <v>0.3345491000000038</v>
       </c>
     </row>
     <row r="159">
@@ -7568,7 +7592,7 @@
         <v>0.5852979171129793</v>
       </c>
       <c r="N159" t="n">
-        <v>0.3071322000000123</v>
+        <v>0.3229627999999991</v>
       </c>
       <c r="O159" t="n">
         <v>11.83865318757962</v>
@@ -7595,7 +7619,7 @@
         <v>40.10056931176479</v>
       </c>
       <c r="X159" t="n">
-        <v>0.2301530000000014</v>
+        <v>0.2225214999999992</v>
       </c>
     </row>
     <row r="160">
@@ -7636,7 +7660,7 @@
         <v>0.6356883051023298</v>
       </c>
       <c r="N160" t="n">
-        <v>0.3004935999999816</v>
+        <v>0.328425100000004</v>
       </c>
       <c r="O160" t="n">
         <v>8.323443435012083</v>
@@ -7663,7 +7687,7 @@
         <v>51.07639331682878</v>
       </c>
       <c r="X160" t="n">
-        <v>0.9245102000000145</v>
+        <v>1.085565600000024</v>
       </c>
     </row>
     <row r="161">
@@ -7707,7 +7731,7 @@
         <v>49.04768695223601</v>
       </c>
       <c r="X161" t="n">
-        <v>0.1571509999999989</v>
+        <v>0.1594564999999761</v>
       </c>
     </row>
     <row r="162">
@@ -7799,7 +7823,7 @@
         <v>0.6209933235511053</v>
       </c>
       <c r="N165" t="n">
-        <v>0.3727388000000076</v>
+        <v>0.3978271000000007</v>
       </c>
     </row>
     <row r="166">
@@ -7840,7 +7864,7 @@
         <v>0.9462813758820232</v>
       </c>
       <c r="N166" t="n">
-        <v>0.2845379999999977</v>
+        <v>0.3051130000000057</v>
       </c>
       <c r="O166" t="n">
         <v>10.6383309008199</v>
@@ -7867,7 +7891,7 @@
         <v>55.91784341088191</v>
       </c>
       <c r="X166" t="n">
-        <v>0.3451438000000167</v>
+        <v>0.4729220000000112</v>
       </c>
     </row>
     <row r="167">
@@ -7908,7 +7932,7 @@
         <v>0.7603749609117307</v>
       </c>
       <c r="N167" t="n">
-        <v>0.3894219000000021</v>
+        <v>0.3664281000000074</v>
       </c>
       <c r="O167" t="n">
         <v>14.5116895743758</v>
@@ -7935,7 +7959,7 @@
         <v>50.05615155655209</v>
       </c>
       <c r="X167" t="n">
-        <v>0.4359570000000019</v>
+        <v>0.4183556000000124</v>
       </c>
     </row>
     <row r="168">
@@ -7979,7 +8003,7 @@
         <v>47.2215047488217</v>
       </c>
       <c r="X168" t="n">
-        <v>0.1991127999999946</v>
+        <v>0.1952605000000176</v>
       </c>
     </row>
     <row r="169">
@@ -8037,7 +8061,7 @@
         <v>0.7472020181523734</v>
       </c>
       <c r="N170" t="n">
-        <v>0.3630362999999761</v>
+        <v>0.3836349000000041</v>
       </c>
       <c r="O170" t="n">
         <v>5.478396406713053</v>
@@ -8064,7 +8088,7 @@
         <v>53.52217043616918</v>
       </c>
       <c r="X170" t="n">
-        <v>1.453104999999994</v>
+        <v>1.387402599999973</v>
       </c>
     </row>
     <row r="171">
@@ -8108,7 +8132,7 @@
         <v>44.46932984274122</v>
       </c>
       <c r="X171" t="n">
-        <v>0.4729230000000086</v>
+        <v>0.3755290999999943</v>
       </c>
     </row>
     <row r="172">
@@ -8183,7 +8207,7 @@
         <v>0.7778893114193726</v>
       </c>
       <c r="N174" t="n">
-        <v>0.2659820000000082</v>
+        <v>0.26204180000002</v>
       </c>
       <c r="O174" t="n">
         <v>7.33544605418831</v>
@@ -8210,7 +8234,7 @@
         <v>45.91439382765128</v>
       </c>
       <c r="X174" t="n">
-        <v>0.1469196000000181</v>
+        <v>0.14005259999999</v>
       </c>
     </row>
     <row r="175">
@@ -8251,7 +8275,7 @@
         <v>0.7129290938553247</v>
       </c>
       <c r="N175" t="n">
-        <v>0.2517746000000045</v>
+        <v>0.3684030000000007</v>
       </c>
       <c r="O175" t="n">
         <v>7.600006853986591</v>
@@ -8278,7 +8302,7 @@
         <v>45.7235754559498</v>
       </c>
       <c r="X175" t="n">
-        <v>0.1610359000000017</v>
+        <v>0.1715643999999656</v>
       </c>
     </row>
     <row r="176">
@@ -8319,7 +8343,7 @@
         <v>0.8156080528736385</v>
       </c>
       <c r="N176" t="n">
-        <v>0.2522821000000022</v>
+        <v>0.2748610999999528</v>
       </c>
       <c r="O176" t="n">
         <v>12.39329015034472</v>
@@ -8346,7 +8370,7 @@
         <v>15.89391891279195</v>
       </c>
       <c r="X176" t="n">
-        <v>0.3014113999999779</v>
+        <v>0.3381062999999926</v>
       </c>
     </row>
     <row r="177">
@@ -8390,7 +8414,7 @@
         <v>49.87619890382092</v>
       </c>
       <c r="X177" t="n">
-        <v>0.1746709999999894</v>
+        <v>0.1789115999999922</v>
       </c>
     </row>
     <row r="178">
@@ -8434,7 +8458,7 @@
         <v>59.1777193867224</v>
       </c>
       <c r="X178" t="n">
-        <v>0.2832932999999969</v>
+        <v>0.2894951999999762</v>
       </c>
     </row>
     <row r="179">
@@ -8475,7 +8499,7 @@
         <v>0.7048534295841888</v>
       </c>
       <c r="N179" t="n">
-        <v>0.4488877000000002</v>
+        <v>0.3166143000000261</v>
       </c>
       <c r="O179" t="n">
         <v>6.689709649957851</v>
@@ -8502,7 +8526,7 @@
         <v>52.44440852385327</v>
       </c>
       <c r="X179" t="n">
-        <v>0.224452499999984</v>
+        <v>0.300763800000027</v>
       </c>
     </row>
     <row r="180">
@@ -8543,7 +8567,7 @@
         <v>0.5422282935131407</v>
       </c>
       <c r="N180" t="n">
-        <v>0.5782371999999896</v>
+        <v>0.5868073999999979</v>
       </c>
     </row>
     <row r="181">
@@ -8584,7 +8608,7 @@
         <v>0.6283519641922324</v>
       </c>
       <c r="N181" t="n">
-        <v>0.2718224000000191</v>
+        <v>0.2848603999999568</v>
       </c>
     </row>
     <row r="182">
@@ -8625,7 +8649,7 @@
         <v>0.814099281542769</v>
       </c>
       <c r="N182" t="n">
-        <v>0.2311184000000139</v>
+        <v>0.245665200000019</v>
       </c>
       <c r="O182" t="n">
         <v>13.74362510448655</v>
@@ -8652,7 +8676,7 @@
         <v>35.02838061829215</v>
       </c>
       <c r="X182" t="n">
-        <v>0.4436105999999995</v>
+        <v>0.4595891000000165</v>
       </c>
     </row>
     <row r="183">
@@ -8710,7 +8734,7 @@
         <v>0.572575338807719</v>
       </c>
       <c r="N184" t="n">
-        <v>0.2805483999999865</v>
+        <v>0.2477547999999956</v>
       </c>
     </row>
     <row r="185">
@@ -8754,7 +8778,7 @@
         <v>40.08249783381137</v>
       </c>
       <c r="X185" t="n">
-        <v>0.2368785000000457</v>
+        <v>0.2314552999999933</v>
       </c>
     </row>
     <row r="186">
@@ -8798,7 +8822,7 @@
         <v>31.25903791033352</v>
       </c>
       <c r="X186" t="n">
-        <v>0.1970769000000132</v>
+        <v>0.2402927999999633</v>
       </c>
     </row>
     <row r="187">
@@ -8839,7 +8863,7 @@
         <v>0.6090177363515266</v>
       </c>
       <c r="N187" t="n">
-        <v>1.126889100000028</v>
+        <v>1.194846499999983</v>
       </c>
       <c r="O187" t="n">
         <v>16.02846480082625</v>
@@ -8866,7 +8890,7 @@
         <v>56.29129486229522</v>
       </c>
       <c r="X187" t="n">
-        <v>0.1846082999999794</v>
+        <v>0.1935507999999686</v>
       </c>
     </row>
     <row r="188">
@@ -8907,7 +8931,7 @@
         <v>0.7505504670917696</v>
       </c>
       <c r="N188" t="n">
-        <v>0.2891850999999974</v>
+        <v>0.2940143000000148</v>
       </c>
       <c r="O188" t="n">
         <v>12.61238131548211</v>
@@ -8934,7 +8958,7 @@
         <v>34.77992114627597</v>
       </c>
       <c r="X188" t="n">
-        <v>0.1756368000000066</v>
+        <v>0.1731376999999839</v>
       </c>
     </row>
     <row r="189">
@@ -8978,7 +9002,7 @@
         <v>51.7118211970843</v>
       </c>
       <c r="X189" t="n">
-        <v>0.5086716999999794</v>
+        <v>0.4769716999999787</v>
       </c>
     </row>
     <row r="190">
@@ -9019,7 +9043,7 @@
         <v>0.6863154554326605</v>
       </c>
       <c r="N190" t="n">
-        <v>0.2912193999999886</v>
+        <v>0.2894448000000125</v>
       </c>
     </row>
     <row r="191">
@@ -9060,7 +9084,7 @@
         <v>0.6236299671445056</v>
       </c>
       <c r="N191" t="n">
-        <v>0.3189706000000001</v>
+        <v>0.3378040000000055</v>
       </c>
       <c r="O191" t="n">
         <v>9.625332320788159</v>
@@ -9084,7 +9108,7 @@
         <v>16.75456998731744</v>
       </c>
       <c r="X191" t="n">
-        <v>0.2628634000000147</v>
+        <v>0.2558223000000339</v>
       </c>
     </row>
     <row r="192">
@@ -9142,7 +9166,7 @@
         <v>0.6519022263066028</v>
       </c>
       <c r="N193" t="n">
-        <v>0.9212594999999624</v>
+        <v>0.947663499999976</v>
       </c>
       <c r="O193" t="n">
         <v>5.216687189586056</v>
@@ -9169,7 +9193,7 @@
         <v>58.08918250403576</v>
       </c>
       <c r="X193" t="n">
-        <v>0.2029987000000233</v>
+        <v>0.2023867999999993</v>
       </c>
     </row>
     <row r="194">
@@ -9210,7 +9234,7 @@
         <v>0.6991461269116794</v>
       </c>
       <c r="N194" t="n">
-        <v>0.2897601999999893</v>
+        <v>0.3060252000000219</v>
       </c>
       <c r="O194" t="n">
         <v>13.20762461494212</v>
@@ -9237,7 +9261,7 @@
         <v>35.86478916565011</v>
       </c>
       <c r="X194" t="n">
-        <v>0.3922673000000145</v>
+        <v>0.4032006999999567</v>
       </c>
     </row>
     <row r="195">
@@ -9278,7 +9302,7 @@
         <v>0.6734162523265559</v>
       </c>
       <c r="N195" t="n">
-        <v>0.781216900000004</v>
+        <v>0.6944995999999719</v>
       </c>
       <c r="O195" t="n">
         <v>6.4533509661202</v>
@@ -9305,7 +9329,7 @@
         <v>44.44825355494731</v>
       </c>
       <c r="X195" t="n">
-        <v>0.3883758000000057</v>
+        <v>0.3851657000000159</v>
       </c>
     </row>
     <row r="196">
@@ -9366,7 +9390,7 @@
         <v>31.99759926785424</v>
       </c>
       <c r="X197" t="n">
-        <v>0.1544418999999948</v>
+        <v>0.1967976999999905</v>
       </c>
     </row>
     <row r="198">
@@ -9407,7 +9431,7 @@
         <v>0.6447031392336856</v>
       </c>
       <c r="N198" t="n">
-        <v>0.8941963000000328</v>
+        <v>0.975314400000002</v>
       </c>
     </row>
     <row r="199">
@@ -9448,7 +9472,7 @@
         <v>0.5760591443043799</v>
       </c>
       <c r="N199" t="n">
-        <v>1.109849999999994</v>
+        <v>1.152804000000003</v>
       </c>
       <c r="O199" t="n">
         <v>11.15054723768442</v>
@@ -9475,7 +9499,7 @@
         <v>52.23679605371535</v>
       </c>
       <c r="X199" t="n">
-        <v>0.2250229999999647</v>
+        <v>0.2464568000000327</v>
       </c>
     </row>
     <row r="200">
@@ -9519,7 +9543,7 @@
         <v>41.06823991440251</v>
       </c>
       <c r="X200" t="n">
-        <v>0.2708096000000069</v>
+        <v>0.2791573000000085</v>
       </c>
     </row>
     <row r="201">
@@ -9563,7 +9587,7 @@
         <v>41.10933814146318</v>
       </c>
       <c r="X201" t="n">
-        <v>0.4713590000000067</v>
+        <v>0.4372706000000335</v>
       </c>
     </row>
     <row r="202">
@@ -9604,7 +9628,7 @@
         <v>0.782415012994204</v>
       </c>
       <c r="N202" t="n">
-        <v>0.3690368000000035</v>
+        <v>0.3872579000000087</v>
       </c>
     </row>
     <row r="203">
@@ -9662,7 +9686,7 @@
         <v>0.503557118560361</v>
       </c>
       <c r="N204" t="n">
-        <v>0.7463981000000217</v>
+        <v>0.7676783</v>
       </c>
     </row>
     <row r="205">
@@ -9703,7 +9727,7 @@
         <v>0.5438033381585889</v>
       </c>
       <c r="N205" t="n">
-        <v>0.3920678999999723</v>
+        <v>0.4191811999999686</v>
       </c>
       <c r="O205" t="n">
         <v>8.275524047001236</v>
@@ -9730,7 +9754,7 @@
         <v>44.28155390322712</v>
       </c>
       <c r="X205" t="n">
-        <v>0.4608219000000418</v>
+        <v>0.4541537999999719</v>
       </c>
     </row>
     <row r="206">
@@ -9771,7 +9795,7 @@
         <v>0.7207876541638537</v>
       </c>
       <c r="N206" t="n">
-        <v>0.234814799999981</v>
+        <v>0.2572161999999594</v>
       </c>
       <c r="O206" t="n">
         <v>12.93941500037211</v>
@@ -9798,7 +9822,7 @@
         <v>38.2256305804159</v>
       </c>
       <c r="X206" t="n">
-        <v>0.6048597999999856</v>
+        <v>0.6338910000000055</v>
       </c>
     </row>
     <row r="207">
@@ -9839,7 +9863,7 @@
         <v>0.7614454848345248</v>
       </c>
       <c r="N207" t="n">
-        <v>0.3686116000000084</v>
+        <v>0.3494547999999895</v>
       </c>
       <c r="O207" t="n">
         <v>17.86380172625017</v>
@@ -9866,7 +9890,7 @@
         <v>32.14037721232523</v>
       </c>
       <c r="X207" t="n">
-        <v>0.327067100000022</v>
+        <v>0.3228742999999668</v>
       </c>
     </row>
     <row r="208">
@@ -9907,7 +9931,7 @@
         <v>0.7850982936704513</v>
       </c>
       <c r="N208" t="n">
-        <v>0.3092391999999791</v>
+        <v>0.3128672000000279</v>
       </c>
       <c r="O208" t="n">
         <v>8.685343267640484</v>
@@ -9934,7 +9958,7 @@
         <v>41.45273931922247</v>
       </c>
       <c r="X208" t="n">
-        <v>0.3053113999999937</v>
+        <v>0.3293914999999856</v>
       </c>
     </row>
     <row r="209">
@@ -9975,7 +9999,7 @@
         <v>0.5801759708679762</v>
       </c>
       <c r="N209" t="n">
-        <v>0.4019395999999915</v>
+        <v>0.4052573999999822</v>
       </c>
       <c r="O209" t="n">
         <v>7.713577086904683</v>
@@ -10002,7 +10026,7 @@
         <v>52.45552571319683</v>
       </c>
       <c r="X209" t="n">
-        <v>0.9513299999999845</v>
+        <v>0.9695361000000275</v>
       </c>
     </row>
     <row r="210">
@@ -10043,7 +10067,7 @@
         <v>0.6433097552103763</v>
       </c>
       <c r="N210" t="n">
-        <v>0.86389029999998</v>
+        <v>0.9286073999999758</v>
       </c>
       <c r="O210" t="n">
         <v>5.789287178664564</v>
@@ -10070,7 +10094,7 @@
         <v>36.24008230675787</v>
       </c>
       <c r="X210" t="n">
-        <v>0.1210042999999814</v>
+        <v>0.1258783000000108</v>
       </c>
     </row>
     <row r="211">
@@ -10111,7 +10135,7 @@
         <v>0.7077004049317255</v>
       </c>
       <c r="N211" t="n">
-        <v>0.3974176999999486</v>
+        <v>0.2944687000000386</v>
       </c>
       <c r="O211" t="n">
         <v>10.88197860710382</v>
@@ -10138,7 +10162,7 @@
         <v>55.39376284974031</v>
       </c>
       <c r="X211" t="n">
-        <v>0.3746679000000199</v>
+        <v>0.3608760000000188</v>
       </c>
     </row>
     <row r="212">
@@ -10233,7 +10257,7 @@
         <v>56.55405614171275</v>
       </c>
       <c r="X215" t="n">
-        <v>0.414815400000009</v>
+        <v>0.4187296999999717</v>
       </c>
     </row>
     <row r="216">
@@ -10274,7 +10298,7 @@
         <v>0.6078827981757445</v>
       </c>
       <c r="N216" t="n">
-        <v>0.3144594000000325</v>
+        <v>0.3144427999999948</v>
       </c>
       <c r="O216" t="n">
         <v>8.853002355128242</v>
@@ -10301,7 +10325,7 @@
         <v>43.54504166427375</v>
       </c>
       <c r="X216" t="n">
-        <v>0.1118285000000014</v>
+        <v>0.1140785999999707</v>
       </c>
     </row>
     <row r="217">
@@ -10342,7 +10366,7 @@
         <v>0.7183214183995025</v>
       </c>
       <c r="N217" t="n">
-        <v>0.2364819999999668</v>
+        <v>0.2549002000000087</v>
       </c>
       <c r="O217" t="n">
         <v>3.46310111957435</v>
@@ -10366,7 +10390,7 @@
         <v>50.46704197121431</v>
       </c>
       <c r="X217" t="n">
-        <v>1.407641000000012</v>
+        <v>1.473101299999996</v>
       </c>
     </row>
     <row r="218">
@@ -10410,7 +10434,7 @@
         <v>52.53270519824861</v>
       </c>
       <c r="X218" t="n">
-        <v>0.2803706000000261</v>
+        <v>0.27221899999995</v>
       </c>
     </row>
     <row r="219">
@@ -10454,7 +10478,7 @@
         <v>41.11439435217051</v>
       </c>
       <c r="X219" t="n">
-        <v>0.2132490999999845</v>
+        <v>0.217903500000034</v>
       </c>
     </row>
     <row r="220">
@@ -10580,7 +10604,7 @@
         <v>0.7480150249470665</v>
       </c>
       <c r="N225" t="n">
-        <v>0.4479420000000118</v>
+        <v>0.4603488000000198</v>
       </c>
       <c r="O225" t="n">
         <v>11.32248837693816</v>
@@ -10607,7 +10631,7 @@
         <v>54.81975454632305</v>
       </c>
       <c r="X225" t="n">
-        <v>0.4586714000000143</v>
+        <v>0.447131000000013</v>
       </c>
     </row>
     <row r="226">
@@ -10648,7 +10672,7 @@
         <v>0.7954285075936763</v>
       </c>
       <c r="N226" t="n">
-        <v>0.2375208000000271</v>
+        <v>0.2526545999999712</v>
       </c>
       <c r="O226" t="n">
         <v>12.00675460680065</v>
@@ -10675,7 +10699,7 @@
         <v>22.1569853107398</v>
       </c>
       <c r="X226" t="n">
-        <v>0.2804884999999899</v>
+        <v>0.2507808999999952</v>
       </c>
     </row>
     <row r="227">
@@ -10719,7 +10743,7 @@
         <v>50.64256292884659</v>
       </c>
       <c r="X227" t="n">
-        <v>0.3056950999999799</v>
+        <v>0.2578683999999498</v>
       </c>
     </row>
     <row r="228">
@@ -10760,7 +10784,7 @@
         <v>0.8316444744474988</v>
       </c>
       <c r="N228" t="n">
-        <v>0.3355225999999902</v>
+        <v>0.3472840000000019</v>
       </c>
       <c r="O228" t="n">
         <v>14.14308152436669</v>
@@ -10787,7 +10811,7 @@
         <v>44.06370669845751</v>
       </c>
       <c r="X228" t="n">
-        <v>0.2130937999999674</v>
+        <v>0.2081701999999837</v>
       </c>
     </row>
     <row r="229">
@@ -10831,7 +10855,7 @@
         <v>41.55535421956677</v>
       </c>
       <c r="X229" t="n">
-        <v>0.1556381999999985</v>
+        <v>0.1600693000000319</v>
       </c>
     </row>
     <row r="230">
@@ -10889,7 +10913,7 @@
         <v>0.5299909355820348</v>
       </c>
       <c r="N231" t="n">
-        <v>0.2266840999999999</v>
+        <v>0.246168799999964</v>
       </c>
       <c r="O231" t="n">
         <v>3.807943758671646</v>
@@ -10916,7 +10940,7 @@
         <v>31.70931821363479</v>
       </c>
       <c r="X231" t="n">
-        <v>0.1029376000000184</v>
+        <v>0.1040482999999881</v>
       </c>
     </row>
     <row r="232">
@@ -10974,7 +10998,7 @@
         <v>0.7456745576053355</v>
       </c>
       <c r="N233" t="n">
-        <v>0.2615996999999766</v>
+        <v>0.2695393000000195</v>
       </c>
       <c r="O233" t="n">
         <v>13.58829959015713</v>
@@ -11001,7 +11025,7 @@
         <v>53.45936777484468</v>
       </c>
       <c r="X233" t="n">
-        <v>0.2347188999999616</v>
+        <v>0.32542490000003</v>
       </c>
     </row>
     <row r="234">
@@ -11042,7 +11066,7 @@
         <v>0.6551296709362725</v>
       </c>
       <c r="N234" t="n">
-        <v>0.4444072999999662</v>
+        <v>0.3485865000000103</v>
       </c>
     </row>
     <row r="235">
@@ -11083,7 +11107,7 @@
         <v>0.7544759929895687</v>
       </c>
       <c r="N235" t="n">
-        <v>0.3506279000000063</v>
+        <v>0.389344699999981</v>
       </c>
     </row>
     <row r="236">
@@ -11141,7 +11165,7 @@
         <v>0.6973238519931545</v>
       </c>
       <c r="N237" t="n">
-        <v>0.3169968000000267</v>
+        <v>0.3460289000000216</v>
       </c>
       <c r="O237" t="n">
         <v>7.066212521311115</v>
@@ -11168,7 +11192,7 @@
         <v>48.660419729311</v>
       </c>
       <c r="X237" t="n">
-        <v>0.1994896999999582</v>
+        <v>0.2225746000000299</v>
       </c>
     </row>
     <row r="238">
@@ -11206,7 +11230,7 @@
         <v>47.45897914785075</v>
       </c>
       <c r="X238" t="n">
-        <v>0.2569255999999882</v>
+        <v>0.2784915999999953</v>
       </c>
     </row>
     <row r="239">
@@ -11247,7 +11271,7 @@
         <v>0.5198072735514186</v>
       </c>
       <c r="N239" t="n">
-        <v>0.2940649999999891</v>
+        <v>0.35134579999999</v>
       </c>
       <c r="O239" t="n">
         <v>11.77171525468184</v>
@@ -11274,7 +11298,7 @@
         <v>46.30647699894831</v>
       </c>
       <c r="X239" t="n">
-        <v>0.2056920999999647</v>
+        <v>0.2453739000000041</v>
       </c>
     </row>
     <row r="240">
@@ -11332,7 +11356,7 @@
         <v>0.7729427953021996</v>
       </c>
       <c r="N241" t="n">
-        <v>0.5724068000000102</v>
+        <v>0.5726324000000318</v>
       </c>
       <c r="O241" t="n">
         <v>16.88767985816003</v>
@@ -11359,7 +11383,7 @@
         <v>58.73543187174175</v>
       </c>
       <c r="X241" t="n">
-        <v>0.3032224999999471</v>
+        <v>0.3533102999999755</v>
       </c>
     </row>
     <row r="242">
@@ -11400,7 +11424,7 @@
         <v>0.5135217450418931</v>
       </c>
       <c r="N242" t="n">
-        <v>0.2731271000000106</v>
+        <v>0.2965318999999909</v>
       </c>
       <c r="O242" t="n">
         <v>8.642245936020171</v>
@@ -11427,7 +11451,7 @@
         <v>10.51377780172834</v>
       </c>
       <c r="X242" t="n">
-        <v>0.1549317999999857</v>
+        <v>0.1583391000000347</v>
       </c>
     </row>
     <row r="243">
@@ -11471,7 +11495,7 @@
         <v>44.91580328599429</v>
       </c>
       <c r="X243" t="n">
-        <v>0.9358550000000037</v>
+        <v>1.067982000000029</v>
       </c>
     </row>
     <row r="244">
@@ -11529,7 +11553,7 @@
         <v>0.5222236691638125</v>
       </c>
       <c r="N245" t="n">
-        <v>0.3167104999999992</v>
+        <v>0.3260050000000092</v>
       </c>
       <c r="O245" t="n">
         <v>10.9526133776974</v>
@@ -11556,7 +11580,7 @@
         <v>50.77072992585659</v>
       </c>
       <c r="X245" t="n">
-        <v>0.2488148999999567</v>
+        <v>0.253162599999996</v>
       </c>
     </row>
     <row r="246">
@@ -11597,7 +11621,7 @@
         <v>0.5999657106355182</v>
       </c>
       <c r="N246" t="n">
-        <v>0.3442885000000047</v>
+        <v>0.2440417000000252</v>
       </c>
       <c r="O246" t="n">
         <v>5.613571937167778</v>
@@ -11624,7 +11648,7 @@
         <v>51.84465779013937</v>
       </c>
       <c r="X246" t="n">
-        <v>0.5346576999999684</v>
+        <v>0.600086000000033</v>
       </c>
     </row>
     <row r="247">
@@ -11665,7 +11689,7 @@
         <v>0.7860287964581961</v>
       </c>
       <c r="N247" t="n">
-        <v>0.300563899999986</v>
+        <v>0.3120013000000199</v>
       </c>
       <c r="O247" t="n">
         <v>6.585357387244891</v>
@@ -11692,7 +11716,7 @@
         <v>35.04845187343415</v>
       </c>
       <c r="X247" t="n">
-        <v>0.1680332999999905</v>
+        <v>0.172411000000011</v>
       </c>
     </row>
     <row r="248">
@@ -11733,7 +11757,7 @@
         <v>0.7386735311150414</v>
       </c>
       <c r="N248" t="n">
-        <v>0.27131270000001</v>
+        <v>0.2979996000000256</v>
       </c>
       <c r="O248" t="n">
         <v>7.159696601410431</v>
@@ -11760,7 +11784,7 @@
         <v>32.09591535847187</v>
       </c>
       <c r="X248" t="n">
-        <v>0.4426563999999757</v>
+        <v>0.4755571999999688</v>
       </c>
     </row>
     <row r="249">
@@ -11801,7 +11825,7 @@
         <v>0.7542459245456868</v>
       </c>
       <c r="N249" t="n">
-        <v>0.3013145000000463</v>
+        <v>0.3187280999999871</v>
       </c>
       <c r="O249" t="n">
         <v>10.38013409313423</v>
@@ -11828,7 +11852,7 @@
         <v>55.83004897783917</v>
       </c>
       <c r="X249" t="n">
-        <v>0.1801580999999715</v>
+        <v>0.2090464999999995</v>
       </c>
     </row>
     <row r="250">
@@ -11869,7 +11893,7 @@
         <v>0.8527506665673604</v>
       </c>
       <c r="N250" t="n">
-        <v>0.2726490000000013</v>
+        <v>0.2821741000000202</v>
       </c>
       <c r="O250" t="n">
         <v>15.83351800973342</v>
@@ -11896,7 +11920,7 @@
         <v>58.44281607161616</v>
       </c>
       <c r="X250" t="n">
-        <v>0.5293929000000048</v>
+        <v>0.4993161000000441</v>
       </c>
     </row>
     <row r="251">
@@ -11937,7 +11961,7 @@
         <v>0.5849756032409672</v>
       </c>
       <c r="N251" t="n">
-        <v>0.2795345999999768</v>
+        <v>0.4407557000000111</v>
       </c>
       <c r="O251" t="n">
         <v>7.861869118386146</v>
@@ -11964,7 +11988,7 @@
         <v>57.68850573345622</v>
       </c>
       <c r="X251" t="n">
-        <v>0.3286970999999994</v>
+        <v>0.3736399000000006</v>
       </c>
     </row>
     <row r="252">
@@ -12005,7 +12029,7 @@
         <v>0.624117025596622</v>
       </c>
       <c r="N252" t="n">
-        <v>0.7009654000000296</v>
+        <v>0.7254422999999974</v>
       </c>
     </row>
     <row r="253">
@@ -12046,7 +12070,7 @@
         <v>0.6419686597652164</v>
       </c>
       <c r="N253" t="n">
-        <v>0.2572674000000461</v>
+        <v>0.2709762999999725</v>
       </c>
     </row>
     <row r="254">
@@ -12090,7 +12114,7 @@
         <v>55.01923652826514</v>
       </c>
       <c r="X254" t="n">
-        <v>0.197306900000001</v>
+        <v>0.2011044999999854</v>
       </c>
     </row>
     <row r="255">
@@ -12131,7 +12155,7 @@
         <v>0.6581219376323464</v>
       </c>
       <c r="N255" t="n">
-        <v>0.8964653999999541</v>
+        <v>0.9486661000000254</v>
       </c>
       <c r="O255" t="n">
         <v>7.689003362713681</v>
@@ -12158,7 +12182,7 @@
         <v>32.56390702090044</v>
       </c>
       <c r="X255" t="n">
-        <v>0.4275357999999869</v>
+        <v>0.4168285999999739</v>
       </c>
     </row>
     <row r="256">
@@ -12199,7 +12223,7 @@
         <v>0.705920964233881</v>
       </c>
       <c r="N256" t="n">
-        <v>0.2995710999999801</v>
+        <v>0.3625000000000114</v>
       </c>
       <c r="O256" t="n">
         <v>7.794572257281294</v>
@@ -12226,7 +12250,7 @@
         <v>35.41513015494758</v>
       </c>
       <c r="X256" t="n">
-        <v>0.1765163999999686</v>
+        <v>0.1864384999999515</v>
       </c>
     </row>
     <row r="257">
@@ -12287,7 +12311,7 @@
         <v>53.83641217865465</v>
       </c>
       <c r="X258" t="n">
-        <v>0.3374512999999979</v>
+        <v>0.3431238999999664</v>
       </c>
     </row>
     <row r="259">
@@ -12328,7 +12352,7 @@
         <v>0.7048733607010829</v>
       </c>
       <c r="N259" t="n">
-        <v>0.3314116999999897</v>
+        <v>0.3507808999999611</v>
       </c>
     </row>
     <row r="260">
@@ -12369,7 +12393,7 @@
         <v>0.667571086807434</v>
       </c>
       <c r="N260" t="n">
-        <v>0.2762708000000202</v>
+        <v>0.2895670000000337</v>
       </c>
     </row>
     <row r="261">
@@ -12410,7 +12434,7 @@
         <v>0.7847440459549182</v>
       </c>
       <c r="N261" t="n">
-        <v>0.301047600000004</v>
+        <v>0.3179309999999873</v>
       </c>
     </row>
     <row r="262">
@@ -12451,7 +12475,7 @@
         <v>0.6182734847249527</v>
       </c>
       <c r="N262" t="n">
-        <v>0.3153757000000041</v>
+        <v>0.3324926999999889</v>
       </c>
     </row>
     <row r="263">
@@ -12526,7 +12550,7 @@
         <v>0.749132990600455</v>
       </c>
       <c r="N265" t="n">
-        <v>0.2726312000000348</v>
+        <v>0.288508400000012</v>
       </c>
       <c r="O265" t="n">
         <v>10.63804465150137</v>
@@ -12553,7 +12577,7 @@
         <v>50.78198565492403</v>
       </c>
       <c r="X265" t="n">
-        <v>0.3138074999999958</v>
+        <v>0.3635677999999984</v>
       </c>
     </row>
     <row r="266">
@@ -12594,7 +12618,7 @@
         <v>0.7926910889900537</v>
       </c>
       <c r="N266" t="n">
-        <v>0.2928449999999998</v>
+        <v>0.3055871999999908</v>
       </c>
     </row>
     <row r="267">
@@ -12652,7 +12676,7 @@
         <v>0.8893562571831392</v>
       </c>
       <c r="N268" t="n">
-        <v>0.2750452999999879</v>
+        <v>0.3048150000000192</v>
       </c>
     </row>
     <row r="269">
@@ -12710,7 +12734,7 @@
         <v>0.780535590502386</v>
       </c>
       <c r="N270" t="n">
-        <v>0.4584494000000063</v>
+        <v>0.4838192999999933</v>
       </c>
     </row>
     <row r="271">
@@ -12751,7 +12775,7 @@
         <v>0.7476205642373706</v>
       </c>
       <c r="N271" t="n">
-        <v>0.2948794000000134</v>
+        <v>0.2972713999999996</v>
       </c>
     </row>
     <row r="272">
@@ -12792,7 +12816,7 @@
         <v>0.5933136613025117</v>
       </c>
       <c r="N272" t="n">
-        <v>0.3176354999999944</v>
+        <v>0.3323232000000189</v>
       </c>
     </row>
     <row r="273">
@@ -12833,7 +12857,7 @@
         <v>0.5579226106722425</v>
       </c>
       <c r="N273" t="n">
-        <v>0.3658491000000481</v>
+        <v>0.3832295999999928</v>
       </c>
       <c r="O273" t="n">
         <v>5.265836946360143</v>
@@ -12860,7 +12884,7 @@
         <v>52.1347451406852</v>
       </c>
       <c r="X273" t="n">
-        <v>0.1952110000000289</v>
+        <v>0.2066065999999864</v>
       </c>
     </row>
     <row r="274">
@@ -12898,7 +12922,7 @@
         <v>57.05277684659177</v>
       </c>
       <c r="X274" t="n">
-        <v>1.323904700000014</v>
+        <v>1.223694699999953</v>
       </c>
     </row>
     <row r="275">
@@ -12939,7 +12963,7 @@
         <v>0.8582887586803196</v>
       </c>
       <c r="N275" t="n">
-        <v>0.4923661000000266</v>
+        <v>0.5157211000000075</v>
       </c>
       <c r="O275" t="n">
         <v>7.863476849427554</v>
@@ -12966,7 +12990,7 @@
         <v>27.58621225378675</v>
       </c>
       <c r="X275" t="n">
-        <v>0.2582126000000358</v>
+        <v>0.2373605000000225</v>
       </c>
     </row>
     <row r="276">
@@ -13041,7 +13065,7 @@
         <v>0.8031583639784863</v>
       </c>
       <c r="N278" t="n">
-        <v>0.2861469000000056</v>
+        <v>0.299398999999994</v>
       </c>
       <c r="O278" t="n">
         <v>9.269626487408967</v>
@@ -13068,7 +13092,7 @@
         <v>50.22548555909117</v>
       </c>
       <c r="X278" t="n">
-        <v>0.4467332000000397</v>
+        <v>0.4042137999999795</v>
       </c>
     </row>
     <row r="279">
@@ -13109,7 +13133,7 @@
         <v>0.622932114668151</v>
       </c>
       <c r="N279" t="n">
-        <v>0.3217149999999833</v>
+        <v>0.3711152000000197</v>
       </c>
       <c r="O279" t="n">
         <v>12.5483241184886</v>
@@ -13136,7 +13160,7 @@
         <v>11.66727437125792</v>
       </c>
       <c r="X279" t="n">
-        <v>0.1703559999999698</v>
+        <v>0.1725684999999544</v>
       </c>
     </row>
     <row r="280">
@@ -13197,7 +13221,7 @@
         <v>58.515930590464</v>
       </c>
       <c r="X281" t="n">
-        <v>0.2089178999999604</v>
+        <v>0.2169630999999868</v>
       </c>
     </row>
     <row r="282">
@@ -13238,7 +13262,7 @@
         <v>0.5586334855331648</v>
       </c>
       <c r="N282" t="n">
-        <v>0.4984788000000435</v>
+        <v>0.5674136999999746</v>
       </c>
       <c r="O282" t="n">
         <v>13.04871656190554</v>
@@ -13265,7 +13289,7 @@
         <v>46.39715553091321</v>
       </c>
       <c r="X282" t="n">
-        <v>1.149377600000037</v>
+        <v>1.347649799999999</v>
       </c>
     </row>
     <row r="283">
@@ -13340,7 +13364,7 @@
         <v>0.8297853709879708</v>
       </c>
       <c r="N285" t="n">
-        <v>0.2959491999999955</v>
+        <v>0.3356944000000226</v>
       </c>
       <c r="O285" t="n">
         <v>15.48882826758408</v>
@@ -13367,7 +13391,7 @@
         <v>44.6819014977566</v>
       </c>
       <c r="X285" t="n">
-        <v>0.2336058999999864</v>
+        <v>0.1932363999999893</v>
       </c>
     </row>
     <row r="286">
@@ -13425,7 +13449,7 @@
         <v>0.5194741443694612</v>
       </c>
       <c r="N287" t="n">
-        <v>0.4784985000000006</v>
+        <v>0.4890558999999826</v>
       </c>
       <c r="O287" t="n">
         <v>14.08542813081427</v>
@@ -13452,7 +13476,7 @@
         <v>58.81957177017364</v>
       </c>
       <c r="X287" t="n">
-        <v>0.1955277000000137</v>
+        <v>0.2365722000000119</v>
       </c>
     </row>
     <row r="288">
@@ -13493,7 +13517,7 @@
         <v>0.7974668826670378</v>
       </c>
       <c r="N288" t="n">
-        <v>0.3453124000000116</v>
+        <v>0.3675513000000024</v>
       </c>
     </row>
     <row r="289">
@@ -13534,7 +13558,7 @@
         <v>0.7950150162254952</v>
       </c>
       <c r="N289" t="n">
-        <v>0.3096918999999616</v>
+        <v>0.3196604999999977</v>
       </c>
       <c r="O289" t="n">
         <v>15.2665675690923</v>
@@ -13561,7 +13585,7 @@
         <v>42.44265984796442</v>
       </c>
       <c r="X289" t="n">
-        <v>0.1642779000000019</v>
+        <v>0.1644281999999748</v>
       </c>
     </row>
     <row r="290">
@@ -13605,7 +13629,7 @@
         <v>46.4404152897402</v>
       </c>
       <c r="X290" t="n">
-        <v>0.5272396000000299</v>
+        <v>0.4996856999999864</v>
       </c>
     </row>
     <row r="291">
@@ -13646,7 +13670,7 @@
         <v>0.7486908851655873</v>
       </c>
       <c r="N291" t="n">
-        <v>0.3749334999999974</v>
+        <v>0.3801703999999972</v>
       </c>
       <c r="O291" t="n">
         <v>12.84654444047575</v>
@@ -13673,7 +13697,7 @@
         <v>57.70163646234255</v>
       </c>
       <c r="X291" t="n">
-        <v>0.6320557000000235</v>
+        <v>0.5598779000000036</v>
       </c>
     </row>
     <row r="292">
@@ -13714,7 +13738,7 @@
         <v>0.8111038024407007</v>
       </c>
       <c r="N292" t="n">
-        <v>0.2226089999999772</v>
+        <v>0.3562934999999925</v>
       </c>
       <c r="O292" t="n">
         <v>4.44372029261366</v>
@@ -13741,7 +13765,7 @@
         <v>59.62019214347447</v>
       </c>
       <c r="X292" t="n">
-        <v>1.99759320000004</v>
+        <v>2.09339650000004</v>
       </c>
     </row>
     <row r="293">
@@ -13782,7 +13806,7 @@
         <v>0.7967663846017742</v>
       </c>
       <c r="N293" t="n">
-        <v>0.2596712000000139</v>
+        <v>0.3129758000000038</v>
       </c>
     </row>
     <row r="294">
@@ -13823,7 +13847,7 @@
         <v>0.5396645747654271</v>
       </c>
       <c r="N294" t="n">
-        <v>0.4854535000000055</v>
+        <v>0.5129622999999697</v>
       </c>
       <c r="O294" t="n">
         <v>3.104462088646399</v>
@@ -13844,7 +13868,7 @@
         <v>58.0197520733285</v>
       </c>
       <c r="X294" t="n">
-        <v>0.953669600000012</v>
+        <v>0.9832636000000434</v>
       </c>
     </row>
     <row r="295">
@@ -13885,7 +13909,7 @@
         <v>0.7582074252020459</v>
       </c>
       <c r="N295" t="n">
-        <v>0.4575738999999999</v>
+        <v>0.4744205000000079</v>
       </c>
       <c r="O295" t="n">
         <v>8.315672261038857</v>
@@ -13912,7 +13936,7 @@
         <v>59.21255483842174</v>
       </c>
       <c r="X295" t="n">
-        <v>0.3303591000000097</v>
+        <v>0.3261297999999897</v>
       </c>
     </row>
     <row r="296">
@@ -13953,7 +13977,7 @@
         <v>0.8660976179885116</v>
       </c>
       <c r="N296" t="n">
-        <v>0.3325820999999678</v>
+        <v>0.3270533000000455</v>
       </c>
       <c r="O296" t="n">
         <v>11.4265202241095</v>
@@ -13980,7 +14004,7 @@
         <v>59.64368308853756</v>
       </c>
       <c r="X296" t="n">
-        <v>0.3094332999999665</v>
+        <v>0.3008378999999763</v>
       </c>
     </row>
     <row r="297">
@@ -14038,7 +14062,7 @@
         <v>0.7302239438641055</v>
       </c>
       <c r="N298" t="n">
-        <v>0.2245608999999718</v>
+        <v>0.2275385000000369</v>
       </c>
       <c r="O298" t="n">
         <v>8.31214379105888</v>
@@ -14065,7 +14089,7 @@
         <v>51.75104565055506</v>
       </c>
       <c r="X298" t="n">
-        <v>0.3191797000000065</v>
+        <v>0.3219595999999569</v>
       </c>
     </row>
     <row r="299">
@@ -14140,7 +14164,7 @@
         <v>0.5764296229561046</v>
       </c>
       <c r="N301" t="n">
-        <v>0.2261900999999966</v>
+        <v>0.2386606000000029</v>
       </c>
       <c r="O301" t="n">
         <v>7.77308427608896</v>
@@ -14167,7 +14191,7 @@
         <v>57.45608137614971</v>
       </c>
       <c r="X301" t="n">
-        <v>0.2465020999999865</v>
+        <v>0.1904559999999833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>